<commit_message>
Nearing a working sheet sync.
</commit_message>
<xml_diff>
--- a/dump-defects.xlsx
+++ b/dump-defects.xlsx
@@ -550,3038 +550,3038 @@
     <row r="2" ht="15" customHeight="1" s="7">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[dfc] 2:1</t>
+          <t>[dfc] 25:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[dfc] 2:2</t>
+          <t>[dfc] 78:95</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[dfc] 2:3</t>
+          <t>[dfc] 82:26</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[dfc] 2:4</t>
+          <t>[dfc] 57:8</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[dfc] 2:5</t>
+          <t>[dfc] 68:42</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[dfc] 2:6</t>
+          <t>[dfc] 95:51</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[dfc] 2:7</t>
+          <t>[dfc] 49:41</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[dfc] 2:8</t>
+          <t>[dfc] 27:72</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[dfc] 2:9</t>
+          <t>[dfc] 61:69</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[dfc] 2:10</t>
+          <t>[dfc] 91:57</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[dfc] 2:11</t>
+          <t>[dfc] 52:12</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[dfc] 2:12</t>
+          <t>[dfc] 35:62</t>
         </is>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="7">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[dfc] 3:1</t>
+          <t>[dfc] 89:20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[dfc] 3:2</t>
+          <t>[dfc] 12:75</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[dfc] 3:3</t>
+          <t>[dfc] 49:81</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[dfc] 3:4</t>
+          <t>[dfc] 14:98</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[dfc] 3:5</t>
+          <t>[dfc] 58:94</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[dfc] 3:6</t>
+          <t>[dfc] 44:12</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[dfc] 3:7</t>
+          <t>[dfc] 95:73</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[dfc] 3:8</t>
+          <t>[dfc] 25:88</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[dfc] 3:9</t>
+          <t>[dfc] 87:41</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[dfc] 3:10</t>
+          <t>[dfc] 62:46</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[dfc] 3:11</t>
+          <t>[dfc] 79:86</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[dfc] 3:12</t>
+          <t>[dfc] 98:37</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="7">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[dfc] 4:1</t>
+          <t>[dfc] 50:63</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[dfc] 4:2</t>
+          <t>[dfc] 66:69</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[dfc] 4:3</t>
+          <t>[dfc] 92:47</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[dfc] 4:4</t>
+          <t>[dfc] 41:17</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[dfc] 4:5</t>
+          <t>[dfc] 51:20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[dfc] 4:6</t>
+          <t>[dfc] 85:13</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[dfc] 4:7</t>
+          <t>[dfc] 62:86</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[dfc] 4:8</t>
+          <t>[dfc] 84:14</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[dfc] 4:9</t>
+          <t>[dfc] 73:71</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[dfc] 4:10</t>
+          <t>[dfc] 56:81</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[dfc] 4:11</t>
+          <t>[dfc] 44:83</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[dfc] 4:12</t>
+          <t>[dfc] 81:18</t>
         </is>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="7">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[dfc] 5:1</t>
+          <t>[dfc] 23:16</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[dfc] 5:2</t>
+          <t>[dfc] 77:48</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[dfc] 5:3</t>
+          <t>[dfc] 25:98</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[dfc] 5:4</t>
+          <t>[dfc] 61:9</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[dfc] 5:5</t>
+          <t>[dfc] 60:53</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[dfc] 5:6</t>
+          <t>[dfc] 88:19</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[dfc] 5:7</t>
+          <t>[dfc] 85:88</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[dfc] 5:8</t>
+          <t>[dfc] 14:66</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[dfc] 5:9</t>
+          <t>[dfc] 39:62</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[dfc] 5:10</t>
+          <t>[dfc] 28:89</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[dfc] 5:11</t>
+          <t>[dfc] 94:46</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[dfc] 5:12</t>
+          <t>[dfc] 99:90</t>
         </is>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="7">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[dfc] 6:1</t>
+          <t>[dfc] 55:16</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[dfc] 6:2</t>
+          <t>[dfc] 29:78</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[dfc] 6:3</t>
+          <t>[dfc] 8:25</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[dfc] 6:4</t>
+          <t>[dfc] 38:21</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[dfc] 6:5</t>
+          <t>[dfc] 79:71</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[dfc] 6:6</t>
+          <t>[dfc] 75:58</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[dfc] 6:7</t>
+          <t>[dfc] 37:89</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[dfc] 6:8</t>
+          <t>[dfc] 72:25</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[dfc] 6:9</t>
+          <t>[dfc] 38:28</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[dfc] 6:10</t>
+          <t>[dfc] 98:39</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[dfc] 6:11</t>
+          <t>[dfc] 7:79</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[dfc] 6:12</t>
+          <t>[dfc] 70:19</t>
         </is>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[dfc] 7:1</t>
+          <t>[dfc] 27:87</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[dfc] 7:2</t>
+          <t>[dfc] 72:15</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[dfc] 7:3</t>
+          <t>[dfc] 15:24</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[dfc] 7:4</t>
+          <t>[dfc] 17:66</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[dfc] 7:5</t>
+          <t>[dfc] 29:15</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[dfc] 7:6</t>
+          <t>[dfc] 25:77</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[dfc] 7:7</t>
+          <t>[dfc] 54:40</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[dfc] 7:8</t>
+          <t>[dfc] 50:15</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[dfc] 7:9</t>
+          <t>[dfc] 83:49</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[dfc] 7:10</t>
+          <t>[dfc] 24:18</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[dfc] 7:11</t>
+          <t>[dfc] 99:34</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[dfc] 7:12</t>
+          <t>[dfc] 40:66</t>
         </is>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" s="7">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[dfc] 8:1</t>
+          <t>[dfc] 58:1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[dfc] 8:2</t>
+          <t>[dfc] 46:20</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[dfc] 8:3</t>
+          <t>[dfc] 97:94</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[dfc] 8:4</t>
+          <t>[dfc] 35:83</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[dfc] 8:5</t>
+          <t>[dfc] 16:79</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[dfc] 8:6</t>
+          <t>[dfc] 34:23</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[dfc] 8:7</t>
+          <t>[dfc] 27:78</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[dfc] 8:8</t>
+          <t>[dfc] 27:27</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[dfc] 8:9</t>
+          <t>[dfc] 52:12</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[dfc] 8:10</t>
+          <t>[dfc] 26:90</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[dfc] 8:11</t>
+          <t>[dfc] 73:69</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[dfc] 8:12</t>
+          <t>[dfc] 10:42</t>
         </is>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" s="7">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[dfc] 9:1</t>
+          <t>[dfc] 85:64</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[dfc] 9:2</t>
+          <t>[dfc] 65:74</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[dfc] 9:3</t>
+          <t>[dfc] 52:3</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[dfc] 9:4</t>
+          <t>[dfc] 71:59</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[dfc] 9:5</t>
+          <t>[dfc] 85:20</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[dfc] 9:6</t>
+          <t>[dfc] 25:79</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[dfc] 9:7</t>
+          <t>[dfc] 89:22</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[dfc] 9:8</t>
+          <t>[dfc] 74:64</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[dfc] 9:9</t>
+          <t>[dfc] 13:35</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[dfc] 9:10</t>
+          <t>[dfc] 16:82</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[dfc] 9:11</t>
+          <t>[dfc] 66:46</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[dfc] 9:12</t>
+          <t>[dfc] 24:16</t>
         </is>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="7">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[dfc] 10:1</t>
+          <t>[dfc] 46:92</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[dfc] 10:2</t>
+          <t>[dfc] 12:55</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[dfc] 10:3</t>
+          <t>[dfc] 69:51</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[dfc] 10:4</t>
+          <t>[dfc] 26:23</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[dfc] 10:5</t>
+          <t>[dfc] 95:68</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[dfc] 10:6</t>
+          <t>[dfc] 57:11</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[dfc] 10:7</t>
+          <t>[dfc] 86:57</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[dfc] 10:8</t>
+          <t>[dfc] 48:77</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>[dfc] 10:9</t>
+          <t>[dfc] 40:59</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[dfc] 10:10</t>
+          <t>[dfc] 85:75</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[dfc] 10:11</t>
+          <t>[dfc] 84:29</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[dfc] 10:12</t>
+          <t>[dfc] 53:90</t>
         </is>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="7">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[dfc] 11:1</t>
+          <t>[dfc] 12:96</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[dfc] 11:2</t>
+          <t>[dfc] 26:40</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[dfc] 11:3</t>
+          <t>[dfc] 86:78</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[dfc] 11:4</t>
+          <t>[dfc] 47:11</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[dfc] 11:5</t>
+          <t>[dfc] 90:33</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[dfc] 11:6</t>
+          <t>[dfc] 88:58</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[dfc] 11:7</t>
+          <t>[dfc] 66:87</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[dfc] 11:8</t>
+          <t>[dfc] 70:61</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[dfc] 11:9</t>
+          <t>[dfc] 34:92</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[dfc] 11:10</t>
+          <t>[dfc] 78:23</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>[dfc] 11:11</t>
+          <t>[dfc] 45:88</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[dfc] 11:12</t>
+          <t>[dfc] 36:66</t>
         </is>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="7">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[dfc] 12:1</t>
+          <t>[dfc] 71:29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[dfc] 12:2</t>
+          <t>[dfc] 82:39</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[dfc] 12:3</t>
+          <t>[dfc] 74:80</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[dfc] 12:4</t>
+          <t>[dfc] 25:86</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[dfc] 12:5</t>
+          <t>[dfc] 51:41</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[dfc] 12:6</t>
+          <t>[dfc] 20:99</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[dfc] 12:7</t>
+          <t>[dfc] 55:47</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>[dfc] 12:8</t>
+          <t>[dfc] 25:17</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[dfc] 12:9</t>
+          <t>[dfc] 85:84</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[dfc] 12:10</t>
+          <t>[dfc] 94:38</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[dfc] 12:11</t>
+          <t>[dfc] 28:44</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>[dfc] 12:12</t>
+          <t>[dfc] 52:59</t>
         </is>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="7">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[dfc] 13:1</t>
+          <t>[dfc] 50:53</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[dfc] 13:2</t>
+          <t>[dfc] 53:33</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[dfc] 13:3</t>
+          <t>[dfc] 99:27</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[dfc] 13:4</t>
+          <t>[dfc] 20:62</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[dfc] 13:5</t>
+          <t>[dfc] 50:74</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[dfc] 13:6</t>
+          <t>[dfc] 66:25</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[dfc] 13:7</t>
+          <t>[dfc] 92:46</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>[dfc] 13:8</t>
+          <t>[dfc] 20:53</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>[dfc] 13:9</t>
+          <t>[dfc] 20:88</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[dfc] 13:10</t>
+          <t>[dfc] 72:59</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>[dfc] 13:11</t>
+          <t>[dfc] 22:12</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>[dfc] 13:12</t>
+          <t>[dfc] 32:40</t>
         </is>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="7">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[dfc] 14:1</t>
+          <t>[dfc] 89:4</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[dfc] 14:2</t>
+          <t>[dfc] 95:21</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[dfc] 14:3</t>
+          <t>[dfc] 23:68</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[dfc] 14:4</t>
+          <t>[dfc] 80:72</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[dfc] 14:5</t>
+          <t>[dfc] 50:59</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[dfc] 14:6</t>
+          <t>[dfc] 65:25</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[dfc] 14:7</t>
+          <t>[dfc] 16:95</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>[dfc] 14:8</t>
+          <t>[dfc] 20:59</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>[dfc] 14:9</t>
+          <t>[dfc] 44:52</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[dfc] 14:10</t>
+          <t>[dfc] 38:26</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[dfc] 14:11</t>
+          <t>[dfc] 89:95</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>[dfc] 14:12</t>
+          <t>[dfc] 73:15</t>
         </is>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="7">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[dfc] 15:1</t>
+          <t>[dfc] 87:26</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[dfc] 15:2</t>
+          <t>[dfc] 41:61</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[dfc] 15:3</t>
+          <t>[dfc] 28:7</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[dfc] 15:4</t>
+          <t>[dfc] 67:93</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[dfc] 15:5</t>
+          <t>[dfc] 17:81</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[dfc] 15:6</t>
+          <t>[dfc] 77:17</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[dfc] 15:7</t>
+          <t>[dfc] 92:10</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>[dfc] 15:8</t>
+          <t>[dfc] 47:89</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[dfc] 15:9</t>
+          <t>[dfc] 88:53</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[dfc] 15:10</t>
+          <t>[dfc] 80:50</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>[dfc] 15:11</t>
+          <t>[dfc] 78:99</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[dfc] 15:12</t>
+          <t>[dfc] 61:36</t>
         </is>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="7">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[dfc] 16:1</t>
+          <t>[dfc] 84:53</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[dfc] 16:2</t>
+          <t>[dfc] 64:60</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[dfc] 16:3</t>
+          <t>[dfc] 76:69</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[dfc] 16:4</t>
+          <t>[dfc] 64:90</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[dfc] 16:5</t>
+          <t>[dfc] 21:30</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[dfc] 16:6</t>
+          <t>[dfc] 91:72</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[dfc] 16:7</t>
+          <t>[dfc] 49:17</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>[dfc] 16:8</t>
+          <t>[dfc] 32:35</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[dfc] 16:9</t>
+          <t>[dfc] 61:61</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>[dfc] 16:10</t>
+          <t>[dfc] 69:12</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>[dfc] 16:11</t>
+          <t>[dfc] 64:30</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[dfc] 16:12</t>
+          <t>[dfc] 95:40</t>
         </is>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="7">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[dfc] 17:1</t>
+          <t>[dfc] 90:57</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[dfc] 17:2</t>
+          <t>[dfc] 83:79</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[dfc] 17:3</t>
+          <t>[dfc] 44:30</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[dfc] 17:4</t>
+          <t>[dfc] 27:36</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[dfc] 17:5</t>
+          <t>[dfc] 91:13</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[dfc] 17:6</t>
+          <t>[dfc] 70:18</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[dfc] 17:7</t>
+          <t>[dfc] 88:68</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>[dfc] 17:8</t>
+          <t>[dfc] 45:93</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[dfc] 17:9</t>
+          <t>[dfc] 91:44</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>[dfc] 17:10</t>
+          <t>[dfc] 85:73</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>[dfc] 17:11</t>
+          <t>[dfc] 30:20</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[dfc] 17:12</t>
+          <t>[dfc] 45:57</t>
         </is>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="7">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[dfc] 18:1</t>
+          <t>[dfc] 70:50</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[dfc] 18:2</t>
+          <t>[dfc] 90:4</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[dfc] 18:3</t>
+          <t>[dfc] 80:86</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[dfc] 18:4</t>
+          <t>[dfc] 69:53</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[dfc] 18:5</t>
+          <t>[dfc] 49:56</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[dfc] 18:6</t>
+          <t>[dfc] 34:57</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[dfc] 18:7</t>
+          <t>[dfc] 71:58</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>[dfc] 18:8</t>
+          <t>[dfc] 89:54</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[dfc] 18:9</t>
+          <t>[dfc] 73:82</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>[dfc] 18:10</t>
+          <t>[dfc] 46:29</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>[dfc] 18:11</t>
+          <t>[dfc] 56:86</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>[dfc] 18:12</t>
+          <t>[dfc] 69:76</t>
         </is>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="7">
       <c r="A19" t="inlineStr">
         <is>
-          <t>[dfc] 19:1</t>
+          <t>[dfc] 65:63</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[dfc] 19:2</t>
+          <t>[dfc] 71:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[dfc] 19:3</t>
+          <t>[dfc] 58:93</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[dfc] 19:4</t>
+          <t>[dfc] 81:23</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[dfc] 19:5</t>
+          <t>[dfc] 76:87</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[dfc] 19:6</t>
+          <t>[dfc] 79:92</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[dfc] 19:7</t>
+          <t>[dfc] 98:90</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>[dfc] 19:8</t>
+          <t>[dfc] 97:50</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[dfc] 19:9</t>
+          <t>[dfc] 52:45</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>[dfc] 19:10</t>
+          <t>[dfc] 93:47</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>[dfc] 19:11</t>
+          <t>[dfc] 80:68</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>[dfc] 19:12</t>
+          <t>[dfc] 99:14</t>
         </is>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="7">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[dfc] 20:1</t>
+          <t>[dfc] 77:70</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[dfc] 20:2</t>
+          <t>[dfc] 58:6</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[dfc] 20:3</t>
+          <t>[dfc] 97:37</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[dfc] 20:4</t>
+          <t>[dfc] 77:21</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[dfc] 20:5</t>
+          <t>[dfc] 88:65</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[dfc] 20:6</t>
+          <t>[dfc] 70:57</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[dfc] 20:7</t>
+          <t>[dfc] 38:78</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>[dfc] 20:8</t>
+          <t>[dfc] 63:83</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>[dfc] 20:9</t>
+          <t>[dfc] 76:51</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>[dfc] 20:10</t>
+          <t>[dfc] 23:32</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>[dfc] 20:11</t>
+          <t>[dfc] 59:27</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>[dfc] 20:12</t>
+          <t>[dfc] 83:96</t>
         </is>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="7">
       <c r="A21" t="inlineStr">
         <is>
-          <t>[dfc] 21:1</t>
+          <t>[dfc] 80:45</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[dfc] 21:2</t>
+          <t>[dfc] 90:60</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[dfc] 21:3</t>
+          <t>[dfc] 74:56</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[dfc] 21:4</t>
+          <t>[dfc] 25:78</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[dfc] 21:5</t>
+          <t>[dfc] 61:69</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[dfc] 21:6</t>
+          <t>[dfc] 43:57</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[dfc] 21:7</t>
+          <t>[dfc] 22:92</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>[dfc] 21:8</t>
+          <t>[dfc] 69:77</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>[dfc] 21:9</t>
+          <t>[dfc] 39:99</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>[dfc] 21:10</t>
+          <t>[dfc] 98:43</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>[dfc] 21:11</t>
+          <t>[dfc] 37:14</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>[dfc] 21:12</t>
+          <t>[dfc] 98:15</t>
         </is>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="7">
       <c r="A22" t="inlineStr">
         <is>
-          <t>[dfc] 22:1</t>
+          <t>[dfc] 24:80</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[dfc] 22:2</t>
+          <t>[dfc] 92:81</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[dfc] 22:3</t>
+          <t>[dfc] 64:49</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[dfc] 22:4</t>
+          <t>[dfc] 75:11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[dfc] 22:5</t>
+          <t>[dfc] 75:96</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[dfc] 22:6</t>
+          <t>[dfc] 98:12</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[dfc] 22:7</t>
+          <t>[dfc] 39:53</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>[dfc] 22:8</t>
+          <t>[dfc] 59:40</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>[dfc] 22:9</t>
+          <t>[dfc] 25:99</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>[dfc] 22:10</t>
+          <t>[dfc] 88:59</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>[dfc] 22:11</t>
+          <t>[dfc] 46:87</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>[dfc] 22:12</t>
+          <t>[dfc] 90:13</t>
         </is>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="7">
       <c r="A23" t="inlineStr">
         <is>
-          <t>[dfc] 23:1</t>
+          <t>[dfc] 66:43</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[dfc] 23:2</t>
+          <t>[dfc] 31:30</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[dfc] 23:3</t>
+          <t>[dfc] 64:57</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[dfc] 23:4</t>
+          <t>[dfc] 52:54</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[dfc] 23:5</t>
+          <t>[dfc] 94:45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[dfc] 23:6</t>
+          <t>[dfc] 84:39</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[dfc] 23:7</t>
+          <t>[dfc] 26:9</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>[dfc] 23:8</t>
+          <t>[dfc] 99:70</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>[dfc] 23:9</t>
+          <t>[dfc] 39:26</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>[dfc] 23:10</t>
+          <t>[dfc] 45:84</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>[dfc] 23:11</t>
+          <t>[dfc] 42:48</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>[dfc] 23:12</t>
+          <t>[dfc] 56:61</t>
         </is>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="7">
       <c r="A24" t="inlineStr">
         <is>
-          <t>[dfc] 24:1</t>
+          <t>[dfc] 34:14</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[dfc] 24:2</t>
+          <t>[dfc] 77:35</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[dfc] 24:3</t>
+          <t>[dfc] 27:81</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>[dfc] 24:4</t>
+          <t>[dfc] 78:87</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[dfc] 24:5</t>
+          <t>[dfc] 66:58</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[dfc] 24:6</t>
+          <t>[dfc] 83:20</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[dfc] 24:7</t>
+          <t>[dfc] 56:76</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>[dfc] 24:8</t>
+          <t>[dfc] 75:12</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>[dfc] 24:9</t>
+          <t>[dfc] 49:81</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>[dfc] 24:10</t>
+          <t>[dfc] 92:51</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>[dfc] 24:11</t>
+          <t>[dfc] 95:81</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>[dfc] 24:12</t>
+          <t>[dfc] 39:32</t>
         </is>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="7">
       <c r="A25" t="inlineStr">
         <is>
-          <t>[dfc] 25:1</t>
+          <t>[dfc] 45:97</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[dfc] 25:2</t>
+          <t>[dfc] 81:55</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[dfc] 25:3</t>
+          <t>[dfc] 76:43</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[dfc] 25:4</t>
+          <t>[dfc] 42:59</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[dfc] 25:5</t>
+          <t>[dfc] 55:97</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[dfc] 25:6</t>
+          <t>[dfc] 57:40</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[dfc] 25:7</t>
+          <t>[dfc] 74:30</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>[dfc] 25:8</t>
+          <t>[dfc] 75:13</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>[dfc] 25:9</t>
+          <t>[dfc] 37:22</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>[dfc] 25:10</t>
+          <t>[dfc] 71:15</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>[dfc] 25:11</t>
+          <t>[dfc] 31:64</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>[dfc] 25:12</t>
+          <t>[dfc] 57:44</t>
         </is>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="7">
       <c r="A26" t="inlineStr">
         <is>
-          <t>[dfc] 26:1</t>
+          <t>[dfc] 96:83</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[dfc] 26:2</t>
+          <t>[dfc] 35:79</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[dfc] 26:3</t>
+          <t>[dfc] 65:52</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[dfc] 26:4</t>
+          <t>[dfc] 30:88</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[dfc] 26:5</t>
+          <t>[dfc] 57:37</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[dfc] 26:6</t>
+          <t>[dfc] 97:89</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[dfc] 26:7</t>
+          <t>[dfc] 34:57</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>[dfc] 26:8</t>
+          <t>[dfc] 99:22</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>[dfc] 26:9</t>
+          <t>[dfc] 80:65</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>[dfc] 26:10</t>
+          <t>[dfc] 68:73</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>[dfc] 26:11</t>
+          <t>[dfc] 46:47</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>[dfc] 26:12</t>
+          <t>[dfc] 65:70</t>
         </is>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="7">
       <c r="A27" t="inlineStr">
         <is>
-          <t>[dfc] 27:1</t>
+          <t>[dfc] 89:18</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[dfc] 27:2</t>
+          <t>[dfc] 49:65</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[dfc] 27:3</t>
+          <t>[dfc] 79:42</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[dfc] 27:4</t>
+          <t>[dfc] 93:65</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[dfc] 27:5</t>
+          <t>[dfc] 32:33</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[dfc] 27:6</t>
+          <t>[dfc] 54:59</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[dfc] 27:7</t>
+          <t>[dfc] 46:17</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>[dfc] 27:8</t>
+          <t>[dfc] 32:85</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[dfc] 27:9</t>
+          <t>[dfc] 71:88</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>[dfc] 27:10</t>
+          <t>[dfc] 96:30</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>[dfc] 27:11</t>
+          <t>[dfc] 48:88</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>[dfc] 27:12</t>
+          <t>[dfc] 60:83</t>
         </is>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="7">
       <c r="A28" t="inlineStr">
         <is>
-          <t>[dfc] 28:1</t>
+          <t>[dfc] 32:29</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[dfc] 28:2</t>
+          <t>[dfc] 87:5</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[dfc] 28:3</t>
+          <t>[dfc] 82:51</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[dfc] 28:4</t>
+          <t>[dfc] 33:34</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[dfc] 28:5</t>
+          <t>[dfc] 72:59</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[dfc] 28:6</t>
+          <t>[dfc] 72:14</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[dfc] 28:7</t>
+          <t>[dfc] 76:54</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>[dfc] 28:8</t>
+          <t>[dfc] 78:33</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>[dfc] 28:9</t>
+          <t>[dfc] 89:79</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>[dfc] 28:10</t>
+          <t>[dfc] 33:54</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>[dfc] 28:11</t>
+          <t>[dfc] 52:30</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>[dfc] 28:12</t>
+          <t>[dfc] 42:75</t>
         </is>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="7">
       <c r="A29" t="inlineStr">
         <is>
-          <t>[dfc] 29:1</t>
+          <t>[dfc] 92:14</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[dfc] 29:2</t>
+          <t>[dfc] 70:66</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[dfc] 29:3</t>
+          <t>[dfc] 76:82</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[dfc] 29:4</t>
+          <t>[dfc] 72:93</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[dfc] 29:5</t>
+          <t>[dfc] 57:54</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[dfc] 29:6</t>
+          <t>[dfc] 46:98</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[dfc] 29:7</t>
+          <t>[dfc] 53:14</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>[dfc] 29:8</t>
+          <t>[dfc] 30:85</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>[dfc] 29:9</t>
+          <t>[dfc] 50:98</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>[dfc] 29:10</t>
+          <t>[dfc] 50:90</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>[dfc] 29:11</t>
+          <t>[dfc] 94:48</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>[dfc] 29:12</t>
+          <t>[dfc] 96:73</t>
         </is>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="7">
       <c r="A30" t="inlineStr">
         <is>
-          <t>[dfc] 30:1</t>
+          <t>[dfc] 48:79</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[dfc] 30:2</t>
+          <t>[dfc] 68:84</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[dfc] 30:3</t>
+          <t>[dfc] 56:78</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>[dfc] 30:4</t>
+          <t>[dfc] 91:81</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[dfc] 30:5</t>
+          <t>[dfc] 65:31</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[dfc] 30:6</t>
+          <t>[dfc] 47:91</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[dfc] 30:7</t>
+          <t>[dfc] 64:25</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>[dfc] 30:8</t>
+          <t>[dfc] 99:11</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>[dfc] 30:9</t>
+          <t>[dfc] 71:93</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>[dfc] 30:10</t>
+          <t>[dfc] 90:60</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>[dfc] 30:11</t>
+          <t>[dfc] 53:79</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>[dfc] 30:12</t>
+          <t>[dfc] 33:20</t>
         </is>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="7">
       <c r="A31" t="inlineStr">
         <is>
-          <t>[dfc] 31:1</t>
+          <t>[dfc] 46:54</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[dfc] 31:2</t>
+          <t>[dfc] 43:81</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[dfc] 31:3</t>
+          <t>[dfc] 77:36</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[dfc] 31:4</t>
+          <t>[dfc] 82:79</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[dfc] 31:5</t>
+          <t>[dfc] 54:53</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[dfc] 31:6</t>
+          <t>[dfc] 40:98</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[dfc] 31:7</t>
+          <t>[dfc] 92:41</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>[dfc] 31:8</t>
+          <t>[dfc] 50:34</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>[dfc] 31:9</t>
+          <t>[dfc] 49:57</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>[dfc] 31:10</t>
+          <t>[dfc] 87:10</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>[dfc] 31:11</t>
+          <t>[dfc] 59:77</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>[dfc] 31:12</t>
+          <t>[dfc] 32:96</t>
         </is>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="7">
       <c r="A32" t="inlineStr">
         <is>
-          <t>[dfc] 32:1</t>
+          <t>[dfc] 36:63</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[dfc] 32:2</t>
+          <t>[dfc] 53:40</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[dfc] 32:3</t>
+          <t>[dfc] 68:88</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>[dfc] 32:4</t>
+          <t>[dfc] 43:43</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[dfc] 32:5</t>
+          <t>[dfc] 99:45</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[dfc] 32:6</t>
+          <t>[dfc] 99:94</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[dfc] 32:7</t>
+          <t>[dfc] 90:38</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>[dfc] 32:8</t>
+          <t>[dfc] 63:12</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>[dfc] 32:9</t>
+          <t>[dfc] 85:19</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>[dfc] 32:10</t>
+          <t>[dfc] 39:24</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>[dfc] 32:11</t>
+          <t>[dfc] 95:66</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>[dfc] 32:12</t>
+          <t>[dfc] 73:21</t>
         </is>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="7">
       <c r="A33" t="inlineStr">
         <is>
-          <t>[dfc] 33:1</t>
+          <t>[dfc] 45:10</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[dfc] 33:2</t>
+          <t>[dfc] 66:97</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[dfc] 33:3</t>
+          <t>[dfc] 59:26</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[dfc] 33:4</t>
+          <t>[dfc] 54:18</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[dfc] 33:5</t>
+          <t>[dfc] 49:21</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[dfc] 33:6</t>
+          <t>[dfc] 97:45</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[dfc] 33:7</t>
+          <t>[dfc] 60:86</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>[dfc] 33:8</t>
+          <t>[dfc] 66:40</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>[dfc] 33:9</t>
+          <t>[dfc] 93:54</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>[dfc] 33:10</t>
+          <t>[dfc] 92:42</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>[dfc] 33:11</t>
+          <t>[dfc] 38:33</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>[dfc] 33:12</t>
+          <t>[dfc] 68:24</t>
         </is>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="7">
       <c r="A34" t="inlineStr">
         <is>
-          <t>[dfc] 34:1</t>
+          <t>[dfc] 88:48</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[dfc] 34:2</t>
+          <t>[dfc] 85:34</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[dfc] 34:3</t>
+          <t>[dfc] 74:61</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[dfc] 34:4</t>
+          <t>[dfc] 90:27</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[dfc] 34:5</t>
+          <t>[dfc] 43:86</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[dfc] 34:6</t>
+          <t>[dfc] 94:35</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[dfc] 34:7</t>
+          <t>[dfc] 60:82</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>[dfc] 34:8</t>
+          <t>[dfc] 35:28</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>[dfc] 34:9</t>
+          <t>[dfc] 89:85</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>[dfc] 34:10</t>
+          <t>[dfc] 90:64</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>[dfc] 34:11</t>
+          <t>[dfc] 45:63</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>[dfc] 34:12</t>
+          <t>[dfc] 95:35</t>
         </is>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="7">
       <c r="A35" t="inlineStr">
         <is>
-          <t>[dfc] 35:1</t>
+          <t>[dfc] 71:9</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[dfc] 35:2</t>
+          <t>[dfc] 52:10</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>[dfc] 35:3</t>
+          <t>[dfc] 96:50</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[dfc] 35:4</t>
+          <t>[dfc] 43:84</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[dfc] 35:5</t>
+          <t>[dfc] 69:96</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[dfc] 35:6</t>
+          <t>[dfc] 80:21</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[dfc] 35:7</t>
+          <t>[dfc] 63:86</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>[dfc] 35:8</t>
+          <t>[dfc] 75:92</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>[dfc] 35:9</t>
+          <t>[dfc] 67:49</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>[dfc] 35:10</t>
+          <t>[dfc] 53:90</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>[dfc] 35:11</t>
+          <t>[dfc] 48:99</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>[dfc] 35:12</t>
+          <t>[dfc] 97:77</t>
         </is>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="7">
       <c r="A36" t="inlineStr">
         <is>
-          <t>[dfc] 36:1</t>
+          <t>[dfc] 70:41</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[dfc] 36:2</t>
+          <t>[dfc] 57:23</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[dfc] 36:3</t>
+          <t>[dfc] 37:48</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[dfc] 36:4</t>
+          <t>[dfc] 44:53</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[dfc] 36:5</t>
+          <t>[dfc] 98:39</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[dfc] 36:6</t>
+          <t>[dfc] 93:96</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[dfc] 36:7</t>
+          <t>[dfc] 44:11</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>[dfc] 36:8</t>
+          <t>[dfc] 56:16</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>[dfc] 36:9</t>
+          <t>[dfc] 82:30</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>[dfc] 36:10</t>
+          <t>[dfc] 97:43</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>[dfc] 36:11</t>
+          <t>[dfc] 92:64</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>[dfc] 36:12</t>
+          <t>[dfc] 54:19</t>
         </is>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="7">
       <c r="A37" t="inlineStr">
         <is>
-          <t>[dfc] 37:1</t>
+          <t>[dfc] 96:27</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[dfc] 37:2</t>
+          <t>[dfc] 64:66</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[dfc] 37:3</t>
+          <t>[dfc] 77:93</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[dfc] 37:4</t>
+          <t>[dfc] 98:6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[dfc] 37:5</t>
+          <t>[dfc] 67:9</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[dfc] 37:6</t>
+          <t>[dfc] 60:8</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[dfc] 37:7</t>
+          <t>[dfc] 39:8</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>[dfc] 37:8</t>
+          <t>[dfc] 51:36</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>[dfc] 37:9</t>
+          <t>[dfc] 59:70</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>[dfc] 37:10</t>
+          <t>[dfc] 71:89</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>[dfc] 37:11</t>
+          <t>[dfc] 52:71</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>[dfc] 37:12</t>
+          <t>[dfc] 44:34</t>
         </is>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="7">
       <c r="A38" t="inlineStr">
         <is>
-          <t>[dfc] 38:1</t>
+          <t>[dfc] 79:76</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[dfc] 38:2</t>
+          <t>[dfc] 71:67</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[dfc] 38:3</t>
+          <t>[dfc] 86:83</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[dfc] 38:4</t>
+          <t>[dfc] 86:46</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[dfc] 38:5</t>
+          <t>[dfc] 40:40</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[dfc] 38:6</t>
+          <t>[dfc] 77:37</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[dfc] 38:7</t>
+          <t>[dfc] 52:9</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>[dfc] 38:8</t>
+          <t>[dfc] 73:13</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[dfc] 38:9</t>
+          <t>[dfc] 44:89</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>[dfc] 38:10</t>
+          <t>[dfc] 60:46</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>[dfc] 38:11</t>
+          <t>[dfc] 47:20</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>[dfc] 38:12</t>
+          <t>[dfc] 73:71</t>
         </is>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" s="7">
       <c r="A39" t="inlineStr">
         <is>
-          <t>[dfc] 39:1</t>
+          <t>[dfc] 48:1</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[dfc] 39:2</t>
+          <t>[dfc] 82:85</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[dfc] 39:3</t>
+          <t>[dfc] 98:47</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>[dfc] 39:4</t>
+          <t>[dfc] 67:66</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[dfc] 39:5</t>
+          <t>[dfc] 83:35</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[dfc] 39:6</t>
+          <t>[dfc] 79:17</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[dfc] 39:7</t>
+          <t>[dfc] 66:34</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>[dfc] 39:8</t>
+          <t>[dfc] 67:73</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>[dfc] 39:9</t>
+          <t>[dfc] 50:90</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>[dfc] 39:10</t>
+          <t>[dfc] 41:43</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>[dfc] 39:11</t>
+          <t>[dfc] 79:32</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>[dfc] 39:12</t>
+          <t>[dfc] 82:95</t>
         </is>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="7">
       <c r="A40" t="inlineStr">
         <is>
-          <t>[dfc] 40:1</t>
+          <t>[dfc] 74:30</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[dfc] 40:2</t>
+          <t>[dfc] 43:53</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[dfc] 40:3</t>
+          <t>[dfc] 76:55</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[dfc] 40:4</t>
+          <t>[dfc] 79:85</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[dfc] 40:5</t>
+          <t>[dfc] 60:37</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[dfc] 40:6</t>
+          <t>[dfc] 92:63</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[dfc] 40:7</t>
+          <t>[dfc] 84:12</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>[dfc] 40:8</t>
+          <t>[dfc] 46:92</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>[dfc] 40:9</t>
+          <t>[dfc] 97:63</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>[dfc] 40:10</t>
+          <t>[dfc] 92:80</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>[dfc] 40:11</t>
+          <t>[dfc] 78:25</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>[dfc] 40:12</t>
+          <t>[dfc] 73:46</t>
         </is>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="7">
       <c r="A41" t="inlineStr">
         <is>
-          <t>[dfc] 41:1</t>
+          <t>[dfc] 62:42</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[dfc] 41:2</t>
+          <t>[dfc] 82:38</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[dfc] 41:3</t>
+          <t>[dfc] 86:58</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[dfc] 41:4</t>
+          <t>[dfc] 94:12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[dfc] 41:5</t>
+          <t>[dfc] 97:18</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[dfc] 41:6</t>
+          <t>[dfc] 72:17</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[dfc] 41:7</t>
+          <t>[dfc] 92:32</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>[dfc] 41:8</t>
+          <t>[dfc] 44:53</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>[dfc] 41:9</t>
+          <t>[dfc] 51:36</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>[dfc] 41:10</t>
+          <t>[dfc] 55:71</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>[dfc] 41:11</t>
+          <t>[dfc] 41:17</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>[dfc] 41:12</t>
+          <t>[dfc] 65:26</t>
         </is>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="7">
       <c r="A42" t="inlineStr">
         <is>
-          <t>[dfc] 42:1</t>
+          <t>[dfc] 78:22</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[dfc] 42:2</t>
+          <t>[dfc] 51:95</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[dfc] 42:3</t>
+          <t>[dfc] 90:79</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>[dfc] 42:4</t>
+          <t>[dfc] 88:81</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[dfc] 42:5</t>
+          <t>[dfc] 76:47</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[dfc] 42:6</t>
+          <t>[dfc] 79:59</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[dfc] 42:7</t>
+          <t>[dfc] 43:91</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>[dfc] 42:8</t>
+          <t>[dfc] 91:82</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>[dfc] 42:9</t>
+          <t>[dfc] 67:9</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>[dfc] 42:10</t>
+          <t>[dfc] 80:21</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>[dfc] 42:11</t>
+          <t>[dfc] 95:63</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>[dfc] 42:12</t>
+          <t>[dfc] 56:55</t>
         </is>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="7">
       <c r="A43" t="inlineStr">
         <is>
-          <t>[dfc] 43:1</t>
+          <t>[dfc] 51:26</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[dfc] 43:2</t>
+          <t>[dfc] 49:55</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[dfc] 43:3</t>
+          <t>[dfc] 84:10</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[dfc] 43:4</t>
+          <t>[dfc] 46:46</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[dfc] 43:5</t>
+          <t>[dfc] 89:22</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[dfc] 43:6</t>
+          <t>[dfc] 56:30</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[dfc] 43:7</t>
+          <t>[dfc] 82:19</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>[dfc] 43:8</t>
+          <t>[dfc] 65:63</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>[dfc] 43:9</t>
+          <t>[dfc] 44:24</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>[dfc] 43:10</t>
+          <t>[dfc] 45:51</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>[dfc] 43:11</t>
+          <t>[dfc] 45:25</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>[dfc] 43:12</t>
+          <t>[dfc] 89:55</t>
         </is>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="7">
       <c r="A44" t="inlineStr">
         <is>
-          <t>[dfc] 44:1</t>
+          <t>[dfc] 81:78</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[dfc] 44:2</t>
+          <t>[dfc] 55:3</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[dfc] 44:3</t>
+          <t>[dfc] 85:53</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[dfc] 44:4</t>
+          <t>[dfc] 85:96</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[dfc] 44:5</t>
+          <t>[dfc] 66:17</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[dfc] 44:6</t>
+          <t>[dfc] 85:22</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[dfc] 44:7</t>
+          <t>[dfc] 86:42</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>[dfc] 44:8</t>
+          <t>[dfc] 78:88</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[dfc] 44:9</t>
+          <t>[dfc] 57:61</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>[dfc] 44:10</t>
+          <t>[dfc] 91:13</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>[dfc] 44:11</t>
+          <t>[dfc] 77:55</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>[dfc] 44:12</t>
+          <t>[dfc] 87:42</t>
         </is>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="7">
       <c r="A45" t="inlineStr">
         <is>
-          <t>[dfc] 45:1</t>
+          <t>[dfc] 60:43</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[dfc] 45:2</t>
+          <t>[dfc] 97:57</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[dfc] 45:3</t>
+          <t>[dfc] 57:87</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[dfc] 45:4</t>
+          <t>[dfc] 74:36</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[dfc] 45:5</t>
+          <t>[dfc] 47:12</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[dfc] 45:6</t>
+          <t>[dfc] 88:47</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[dfc] 45:7</t>
+          <t>[dfc] 95:80</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>[dfc] 45:8</t>
+          <t>[dfc] 67:69</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[dfc] 45:9</t>
+          <t>[dfc] 49:29</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>[dfc] 45:10</t>
+          <t>[dfc] 88:26</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>[dfc] 45:11</t>
+          <t>[dfc] 69:99</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>[dfc] 45:12</t>
+          <t>[dfc] 52:99</t>
         </is>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="7">
       <c r="A46" t="inlineStr">
         <is>
-          <t>[dfc] 46:1</t>
+          <t>[dfc] 67:13</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[dfc] 46:2</t>
+          <t>[dfc] 78:75</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[dfc] 46:3</t>
+          <t>[dfc] 87:97</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[dfc] 46:4</t>
+          <t>[dfc] 96:76</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[dfc] 46:5</t>
+          <t>[dfc] 81:36</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[dfc] 46:6</t>
+          <t>[dfc] 46:84</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>[dfc] 46:7</t>
+          <t>[dfc] 46:49</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>[dfc] 46:8</t>
+          <t>[dfc] 86:15</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>[dfc] 46:9</t>
+          <t>[dfc] 77:14</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>[dfc] 46:10</t>
+          <t>[dfc] 56:50</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>[dfc] 46:11</t>
+          <t>[dfc] 57:72</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>[dfc] 46:12</t>
+          <t>[dfc] 65:70</t>
         </is>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="7">
       <c r="A47" t="inlineStr">
         <is>
-          <t>[dfc] 47:1</t>
+          <t>[dfc] 68:81</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[dfc] 47:2</t>
+          <t>[dfc] 76:79</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[dfc] 47:3</t>
+          <t>[dfc] 79:72</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[dfc] 47:4</t>
+          <t>[dfc] 59:43</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[dfc] 47:5</t>
+          <t>[dfc] 68:40</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[dfc] 47:6</t>
+          <t>[dfc] 94:31</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>[dfc] 47:7</t>
+          <t>[dfc] 51:38</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>[dfc] 47:8</t>
+          <t>[dfc] 83:62</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[dfc] 47:9</t>
+          <t>[dfc] 56:61</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>[dfc] 47:10</t>
+          <t>[dfc] 62:83</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>[dfc] 47:11</t>
+          <t>[dfc] 87:52</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>[dfc] 47:12</t>
+          <t>[dfc] 61:88</t>
         </is>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="7">
       <c r="A48" t="inlineStr">
         <is>
-          <t>[dfc] 48:1</t>
+          <t>[dfc] 62:74</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[dfc] 48:2</t>
+          <t>[dfc] 62:96</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[dfc] 48:3</t>
+          <t>[dfc] 50:55</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[dfc] 48:4</t>
+          <t>[dfc] 94:79</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[dfc] 48:5</t>
+          <t>[dfc] 71:18</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[dfc] 48:6</t>
+          <t>[dfc] 96:81</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>[dfc] 48:7</t>
+          <t>[dfc] 69:23</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>[dfc] 48:8</t>
+          <t>[dfc] 97:28</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>[dfc] 48:9</t>
+          <t>[dfc] 88:22</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>[dfc] 48:10</t>
+          <t>[dfc] 55:58</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>[dfc] 48:11</t>
+          <t>[dfc] 77:78</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>[dfc] 48:12</t>
+          <t>[dfc] 80:97</t>
         </is>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="7">
       <c r="A49" t="inlineStr">
         <is>
-          <t>[dfc] 49:1</t>
+          <t>[dfc] 97:19</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[dfc] 49:2</t>
+          <t>[dfc] 83:95</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[dfc] 49:3</t>
+          <t>[dfc] 62:49</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[dfc] 49:4</t>
+          <t>[dfc] 86:14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[dfc] 49:5</t>
+          <t>[dfc] 97:50</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[dfc] 49:6</t>
+          <t>[dfc] 68:46</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[dfc] 49:7</t>
+          <t>[dfc] 83:94</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>[dfc] 49:8</t>
+          <t>[dfc] 88:98</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>[dfc] 49:9</t>
+          <t>[dfc] 70:57</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>[dfc] 49:10</t>
+          <t>[dfc] 55:49</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>[dfc] 49:11</t>
+          <t>[dfc] 83:19</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>[dfc] 49:12</t>
+          <t>[dfc] 66:12</t>
         </is>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="7">
       <c r="A50" t="inlineStr">
         <is>
-          <t>[dfc] 50:1</t>
+          <t>[dfc] 85:31</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[dfc] 50:2</t>
+          <t>[dfc] 84:67</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[dfc] 50:3</t>
+          <t>[dfc] 94:88</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[dfc] 50:4</t>
+          <t>[dfc] 61:32</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[dfc] 50:5</t>
+          <t>[dfc] 71:7</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[dfc] 50:6</t>
+          <t>[dfc] 59:77</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[dfc] 50:7</t>
+          <t>[dfc] 60:77</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>[dfc] 50:8</t>
+          <t>[dfc] 69:75</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>[dfc] 50:9</t>
+          <t>[dfc] 60:51</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>[dfc] 50:10</t>
+          <t>[dfc] 85:82</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>[dfc] 50:11</t>
+          <t>[dfc] 52:26</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>[dfc] 50:12</t>
+          <t>[dfc] 99:80</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Multiple bug fixes now ready to code appending new rows.
</commit_message>
<xml_diff>
--- a/dump-defects.xlsx
+++ b/dump-defects.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hypercare Defects" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hypercare Defects" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -41,19 +41,19 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Cantarell"/>
+      <name val="Ubuntu"/>
       <charset val="1"/>
       <family val="0"/>
       <color rgb="FF000000"/>
-      <sz val="12"/>
+      <sz val="11"/>
     </font>
     <font>
-      <name val="Cantarell"/>
+      <name val="Ubuntu"/>
       <charset val="1"/>
       <family val="0"/>
       <b val="1"/>
       <color rgb="FF000000"/>
-      <sz val="12"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="3">
@@ -89,8 +89,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -105,13 +108,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,3562 +482,3573 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="15.43" customWidth="1" style="4" min="1" max="12"/>
-    <col width="8.529999999999999" customWidth="1" style="4" min="13" max="1024"/>
+    <col width="15" customWidth="1" style="5" min="1" max="1"/>
+    <col width="15" customWidth="1" style="5" min="2" max="12"/>
+    <col width="15" customWidth="1" style="6" min="3" max="3"/>
+    <col width="15" customWidth="1" style="6" min="4" max="4"/>
+    <col width="15" customWidth="1" style="6" min="5" max="5"/>
+    <col width="15" customWidth="1" style="6" min="6" max="6"/>
+    <col width="15" customWidth="1" style="6" min="7" max="7"/>
+    <col width="15" customWidth="1" style="6" min="8" max="8"/>
+    <col width="15" customWidth="1" style="6" min="9" max="9"/>
+    <col width="15" customWidth="1" style="6" min="10" max="10"/>
+    <col width="15" customWidth="1" style="6" min="11" max="11"/>
+    <col width="15" customWidth="1" style="6" min="12" max="12"/>
+    <col width="8.529999999999999" customWidth="1" style="5" min="13" max="1024"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customFormat="1" customHeight="1" s="5">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1" ht="15" customFormat="1" customHeight="1" s="7">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Opened</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Short description</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Impact</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="E1" s="8" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>Urgency</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="H1" s="6" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>Assigned to</t>
         </is>
       </c>
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="8" t="inlineStr">
         <is>
           <t>Requestor</t>
         </is>
       </c>
-      <c r="J1" s="6" t="inlineStr">
+      <c r="J1" s="8" t="inlineStr">
         <is>
           <t>Assignment group</t>
         </is>
       </c>
-      <c r="K1" s="6" t="inlineStr">
+      <c r="K1" s="8" t="inlineStr">
         <is>
           <t>Due date</t>
         </is>
       </c>
-      <c r="L1" s="6" t="inlineStr">
+      <c r="L1" s="8" t="inlineStr">
         <is>
           <t>Rank</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="7">
+    <row r="2" ht="15" customHeight="1" s="6">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[dfc] 25:35</t>
+          <t>[DFC] 950:887</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[dfc] 78:95</t>
+          <t>[DFC] 501:967</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[dfc] 82:26</t>
+          <t>[DFC] 165:570</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[dfc] 57:8</t>
+          <t>[DFC] 269:367</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[dfc] 68:42</t>
+          <t>[DFC] 283:185</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[dfc] 95:51</t>
+          <t>[DFC] 258:450</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[dfc] 49:41</t>
+          <t>[DFC] 566:947</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[dfc] 27:72</t>
+          <t>[DFC] 360:936</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[dfc] 61:69</t>
+          <t>[DFC] 342:611</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[dfc] 91:57</t>
+          <t>[DFC] 485:551</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[dfc] 52:12</t>
+          <t>[DFC] 104:981</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[dfc] 35:62</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="7">
+          <t>[DFC] 112:388</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="6">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[dfc] 89:20</t>
+          <t>[DFC] 327:622</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[dfc] 12:75</t>
+          <t>[DFC] 730:360</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[dfc] 49:81</t>
+          <t>[DFC] 824:323</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[dfc] 14:98</t>
+          <t>[DFC] 127:234</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[dfc] 58:94</t>
+          <t>[DFC] 481:405</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[dfc] 44:12</t>
+          <t>[DFC] 531:636</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[dfc] 95:73</t>
+          <t>[DFC] 562:632</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[dfc] 25:88</t>
+          <t>[DFC] 815:845</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[dfc] 87:41</t>
+          <t>[DFC] 840:130</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[dfc] 62:46</t>
+          <t>[DFC] 490:123</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[dfc] 79:86</t>
+          <t>[DFC] 490:912</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[dfc] 98:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="7">
+          <t>[DFC] 845:122</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="6">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[dfc] 50:63</t>
+          <t>[DFC] 461:977</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[dfc] 66:69</t>
+          <t>[DFC] 882:233</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[dfc] 92:47</t>
+          <t>[DFC] 355:696</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[dfc] 41:17</t>
+          <t>[DFC] 599:785</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[dfc] 51:20</t>
+          <t>[DFC] 444:602</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[dfc] 85:13</t>
+          <t>[DFC] 881:107</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[dfc] 62:86</t>
+          <t>[DFC] 845:667</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[dfc] 84:14</t>
+          <t>[DFC] 511:189</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[dfc] 73:71</t>
+          <t>[DFC] 540:158</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[dfc] 56:81</t>
+          <t>[DFC] 864:513</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[dfc] 44:83</t>
+          <t>[DFC] 895:721</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[dfc] 81:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="7">
+          <t>[DFC] 648:856</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="6">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[dfc] 23:16</t>
+          <t>[DFC] 120:290</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[dfc] 77:48</t>
+          <t>[DFC] 346:153</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[dfc] 25:98</t>
+          <t>[DFC] 996:340</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[dfc] 61:9</t>
+          <t>[DFC] 602:344</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[dfc] 60:53</t>
+          <t>[DFC] 493:138</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[dfc] 88:19</t>
+          <t>[DFC] 110:516</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[dfc] 85:88</t>
+          <t>[DFC] 185:630</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[dfc] 14:66</t>
+          <t>[DFC] 772:295</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[dfc] 39:62</t>
+          <t>[DFC] 458:580</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[dfc] 28:89</t>
+          <t>[DFC] 294:997</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[dfc] 94:46</t>
+          <t>[DFC] 663:151</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[dfc] 99:90</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="7">
+          <t>[DFC] 676:808</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[dfc] 55:16</t>
+          <t>[DFC] 270:848</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[dfc] 29:78</t>
+          <t>[DFC] 124:777</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[dfc] 8:25</t>
+          <t>[DFC] 436:859</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[dfc] 38:21</t>
+          <t>[DFC] 999:848</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[dfc] 79:71</t>
+          <t>[DFC] 394:568</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[dfc] 75:58</t>
+          <t>[DFC] 398:809</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[dfc] 37:89</t>
+          <t>[DFC] 843:462</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[dfc] 72:25</t>
+          <t>[DFC] 883:457</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[dfc] 38:28</t>
+          <t>[DFC] 638:125</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[dfc] 98:39</t>
+          <t>[DFC] 292:471</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[dfc] 7:79</t>
+          <t>[DFC] 811:198</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[dfc] 70:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="7">
+          <t>[DFC] 994:191</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="6">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[dfc] 27:87</t>
+          <t>[DFC] 186:476</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[dfc] 72:15</t>
+          <t>[DFC] 456:616</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[dfc] 15:24</t>
+          <t>[DFC] 134:176</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[dfc] 17:66</t>
+          <t>[DFC] 721:729</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[dfc] 29:15</t>
+          <t>[DFC] 580:988</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[dfc] 25:77</t>
+          <t>[DFC] 249:173</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[dfc] 54:40</t>
+          <t>[DFC] 481:904</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>[dfc] 50:15</t>
+          <t>[DFC] 712:805</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[dfc] 83:49</t>
+          <t>[DFC] 259:898</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[dfc] 24:18</t>
+          <t>[DFC] 688:612</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[dfc] 99:34</t>
+          <t>[DFC] 767:818</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[dfc] 40:66</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="7">
+          <t>[DFC] 739:928</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="6">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[dfc] 58:1</t>
+          <t>[DFC] 258:687</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[dfc] 46:20</t>
+          <t>[DFC] 448:132</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[dfc] 97:94</t>
+          <t>[DFC] 297:393</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[dfc] 35:83</t>
+          <t>[DFC] 401:579</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[dfc] 16:79</t>
+          <t>[DFC] 478:616</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[dfc] 34:23</t>
+          <t>[DFC] 264:304</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[dfc] 27:78</t>
+          <t>[DFC] 770:105</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[dfc] 27:27</t>
+          <t>[DFC] 572:519</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[dfc] 52:12</t>
+          <t>[DFC] 472:340</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[dfc] 26:90</t>
+          <t>[DFC] 389:753</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[dfc] 73:69</t>
+          <t>[DFC] 943:520</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[dfc] 10:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="7">
+          <t>[DFC] 318:335</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="6">
       <c r="A9" t="inlineStr">
         <is>
-          <t>[dfc] 85:64</t>
+          <t>[DFC] 294:609</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[dfc] 65:74</t>
+          <t>[DFC] 508:368</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[dfc] 52:3</t>
+          <t>[DFC] 953:409</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[dfc] 71:59</t>
+          <t>[DFC] 355:708</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[dfc] 85:20</t>
+          <t>[DFC] 873:466</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[dfc] 25:79</t>
+          <t>[DFC] 100:601</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[dfc] 89:22</t>
+          <t>[DFC] 819:389</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[dfc] 74:64</t>
+          <t>[DFC] 980:762</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[dfc] 13:35</t>
+          <t>[DFC] 244:986</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[dfc] 16:82</t>
+          <t>[DFC] 382:332</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[dfc] 66:46</t>
+          <t>[DFC] 109:935</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[dfc] 24:16</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="7">
+          <t>[DFC] 276:540</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="6">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[dfc] 46:92</t>
+          <t>[DFC] 938:931</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[dfc] 12:55</t>
+          <t>[DFC] 836:320</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[dfc] 69:51</t>
+          <t>[DFC] 586:511</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[dfc] 26:23</t>
+          <t>[DFC] 459:488</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[dfc] 95:68</t>
+          <t>[DFC] 772:450</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[dfc] 57:11</t>
+          <t>[DFC] 988:753</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[dfc] 86:57</t>
+          <t>[DFC] 714:952</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[dfc] 48:77</t>
+          <t>[DFC] 241:698</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>[dfc] 40:59</t>
+          <t>[DFC] 981:710</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[dfc] 85:75</t>
+          <t>[DFC] 570:474</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[dfc] 84:29</t>
+          <t>[DFC] 127:942</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[dfc] 53:90</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="7">
+          <t>[DFC] 967:459</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="6">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[dfc] 12:96</t>
+          <t>[DFC] 770:478</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[dfc] 26:40</t>
+          <t>[DFC] 889:357</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[dfc] 86:78</t>
+          <t>[DFC] 723:178</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[dfc] 47:11</t>
+          <t>[DFC] 460:764</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[dfc] 90:33</t>
+          <t>[DFC] 568:567</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[dfc] 88:58</t>
+          <t>[DFC] 461:397</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[dfc] 66:87</t>
+          <t>[DFC] 700:945</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[dfc] 70:61</t>
+          <t>[DFC] 955:176</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>[dfc] 34:92</t>
+          <t>[DFC] 286:758</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[dfc] 78:23</t>
+          <t>[DFC] 490:102</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>[dfc] 45:88</t>
+          <t>[DFC] 797:902</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[dfc] 36:66</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" s="7">
+          <t>[DFC] 956:445</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" s="6">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[dfc] 71:29</t>
+          <t>[DFC] 101:337</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[dfc] 82:39</t>
+          <t>[DFC] 722:381</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[dfc] 74:80</t>
+          <t>[DFC] 297:801</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[dfc] 25:86</t>
+          <t>[DFC] 701:252</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[dfc] 51:41</t>
+          <t>[DFC] 635:803</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[dfc] 20:99</t>
+          <t>[DFC] 604:830</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[dfc] 55:47</t>
+          <t>[DFC] 299:563</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>[dfc] 25:17</t>
+          <t>[DFC] 484:922</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[dfc] 85:84</t>
+          <t>[DFC] 808:966</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[dfc] 94:38</t>
+          <t>[DFC] 849:865</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[dfc] 28:44</t>
+          <t>[DFC] 526:125</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>[dfc] 52:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" s="7">
+          <t>[DFC] 177:211</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" s="6">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[dfc] 50:53</t>
+          <t>[DFC] 209:405</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[dfc] 53:33</t>
+          <t>[DFC] 873:270</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[dfc] 99:27</t>
+          <t>[DFC] 738:628</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[dfc] 20:62</t>
+          <t>[DFC] 432:357</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[dfc] 50:74</t>
+          <t>[DFC] 286:676</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[dfc] 66:25</t>
+          <t>[DFC] 661:355</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[dfc] 92:46</t>
+          <t>[DFC] 669:344</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>[dfc] 20:53</t>
+          <t>[DFC] 863:972</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>[dfc] 20:88</t>
+          <t>[DFC] 863:564</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[dfc] 72:59</t>
+          <t>[DFC] 374:309</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>[dfc] 22:12</t>
+          <t>[DFC] 474:696</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>[dfc] 32:40</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="7">
+          <t>[DFC] 465:934</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="6">
       <c r="A14" t="inlineStr">
         <is>
-          <t>[dfc] 89:4</t>
+          <t>[DFC] 104:255</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[dfc] 95:21</t>
+          <t>[DFC] 373:182</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[dfc] 23:68</t>
+          <t>[DFC] 108:860</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[dfc] 80:72</t>
+          <t>[DFC] 952:347</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[dfc] 50:59</t>
+          <t>[DFC] 293:599</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[dfc] 65:25</t>
+          <t>[DFC] 356:551</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[dfc] 16:95</t>
+          <t>[DFC] 351:780</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>[dfc] 20:59</t>
+          <t>[DFC] 351:914</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>[dfc] 44:52</t>
+          <t>[DFC] 784:157</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[dfc] 38:26</t>
+          <t>[DFC] 486:795</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[dfc] 89:95</t>
+          <t>[DFC] 559:163</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>[dfc] 73:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="7">
+          <t>[DFC] 297:478</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="6">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[dfc] 87:26</t>
+          <t>[DFC] 625:990</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[dfc] 41:61</t>
+          <t>[DFC] 288:262</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[dfc] 28:7</t>
+          <t>[DFC] 474:517</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[dfc] 67:93</t>
+          <t>[DFC] 162:136</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[dfc] 17:81</t>
+          <t>[DFC] 767:370</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[dfc] 77:17</t>
+          <t>[DFC] 413:818</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[dfc] 92:10</t>
+          <t>[DFC] 193:688</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>[dfc] 47:89</t>
+          <t>[DFC] 811:382</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[dfc] 88:53</t>
+          <t>[DFC] 612:113</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[dfc] 80:50</t>
+          <t>[DFC] 600:981</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>[dfc] 78:99</t>
+          <t>[DFC] 672:943</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[dfc] 61:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" s="7">
+          <t>[DFC] 103:767</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" s="6">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[dfc] 84:53</t>
+          <t>[DFC] 852:412</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[dfc] 64:60</t>
+          <t>[DFC] 214:706</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[dfc] 76:69</t>
+          <t>[DFC] 284:915</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[dfc] 64:90</t>
+          <t>[DFC] 234:487</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[dfc] 21:30</t>
+          <t>[DFC] 737:762</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[dfc] 91:72</t>
+          <t>[DFC] 567:387</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[dfc] 49:17</t>
+          <t>[DFC] 106:842</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>[dfc] 32:35</t>
+          <t>[DFC] 967:723</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[dfc] 61:61</t>
+          <t>[DFC] 581:336</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>[dfc] 69:12</t>
+          <t>[DFC] 193:990</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>[dfc] 64:30</t>
+          <t>[DFC] 818:179</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[dfc] 95:40</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" s="7">
+          <t>[DFC] 297:825</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" s="6">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[dfc] 90:57</t>
+          <t>[DFC] 183:861</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[dfc] 83:79</t>
+          <t>[DFC] 845:591</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[dfc] 44:30</t>
+          <t>[DFC] 720:299</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[dfc] 27:36</t>
+          <t>[DFC] 668:400</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[dfc] 91:13</t>
+          <t>[DFC] 265:571</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[dfc] 70:18</t>
+          <t>[DFC] 341:740</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[dfc] 88:68</t>
+          <t>[DFC] 178:978</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>[dfc] 45:93</t>
+          <t>[DFC] 264:857</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[dfc] 91:44</t>
+          <t>[DFC] 928:881</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>[dfc] 85:73</t>
+          <t>[DFC] 310:165</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>[dfc] 30:20</t>
+          <t>[DFC] 130:799</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[dfc] 45:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" s="7">
+          <t>[DFC] 534:948</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" s="6">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[dfc] 70:50</t>
+          <t>[DFC] 776:770</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[dfc] 90:4</t>
+          <t>[DFC] 456:122</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[dfc] 80:86</t>
+          <t>[DFC] 790:841</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[dfc] 69:53</t>
+          <t>[DFC] 948:361</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[dfc] 49:56</t>
+          <t>[DFC] 997:422</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[dfc] 34:57</t>
+          <t>[DFC] 283:389</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[dfc] 71:58</t>
+          <t>[DFC] 472:577</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>[dfc] 89:54</t>
+          <t>[DFC] 665:226</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[dfc] 73:82</t>
+          <t>[DFC] 887:794</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>[dfc] 46:29</t>
+          <t>[DFC] 135:289</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>[dfc] 56:86</t>
+          <t>[DFC] 594:282</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>[dfc] 69:76</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1" s="7">
+          <t>[DFC] 380:910</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1" s="6">
       <c r="A19" t="inlineStr">
         <is>
-          <t>[dfc] 65:63</t>
+          <t>[DFC] 992:763</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[dfc] 71:22</t>
+          <t>[DFC] 417:864</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[dfc] 58:93</t>
+          <t>[DFC] 872:160</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[dfc] 81:23</t>
+          <t>[DFC] 973:307</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[dfc] 76:87</t>
+          <t>[DFC] 536:826</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[dfc] 79:92</t>
+          <t>[DFC] 569:757</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[dfc] 98:90</t>
+          <t>[DFC] 615:366</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>[dfc] 97:50</t>
+          <t>[DFC] 277:155</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[dfc] 52:45</t>
+          <t>[DFC] 168:952</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>[dfc] 93:47</t>
+          <t>[DFC] 648:440</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>[dfc] 80:68</t>
+          <t>[DFC] 553:536</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>[dfc] 99:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1" s="7">
+          <t>[DFC] 852:442</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1" s="6">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[dfc] 77:70</t>
+          <t>[DFC] 668:779</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[dfc] 58:6</t>
+          <t>[DFC] 299:328</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[dfc] 97:37</t>
+          <t>[DFC] 196:607</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[dfc] 77:21</t>
+          <t>[DFC] 606:947</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[dfc] 88:65</t>
+          <t>[DFC] 404:107</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[dfc] 70:57</t>
+          <t>[DFC] 702:932</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[dfc] 38:78</t>
+          <t>[DFC] 718:817</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>[dfc] 63:83</t>
+          <t>[DFC] 407:977</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>[dfc] 76:51</t>
+          <t>[DFC] 397:221</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>[dfc] 23:32</t>
+          <t>[DFC] 469:281</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>[dfc] 59:27</t>
+          <t>[DFC] 432:503</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>[dfc] 83:96</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1" s="7">
+          <t>[DFC] 994:215</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1" s="6">
       <c r="A21" t="inlineStr">
         <is>
-          <t>[dfc] 80:45</t>
+          <t>[DFC] 832:134</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[dfc] 90:60</t>
+          <t>[DFC] 155:492</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[dfc] 74:56</t>
+          <t>[DFC] 889:706</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[dfc] 25:78</t>
+          <t>[DFC] 169:581</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[dfc] 61:69</t>
+          <t>[DFC] 813:838</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[dfc] 43:57</t>
+          <t>[DFC] 433:858</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[dfc] 22:92</t>
+          <t>[DFC] 488:109</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>[dfc] 69:77</t>
+          <t>[DFC] 768:594</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>[dfc] 39:99</t>
+          <t>[DFC] 401:940</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>[dfc] 98:43</t>
+          <t>[DFC] 558:853</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>[dfc] 37:14</t>
+          <t>[DFC] 392:572</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>[dfc] 98:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="15" customHeight="1" s="7">
+          <t>[DFC] 627:934</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1" s="6">
       <c r="A22" t="inlineStr">
         <is>
-          <t>[dfc] 24:80</t>
+          <t>[DFC] 703:311</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[dfc] 92:81</t>
+          <t>[DFC] 340:599</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[dfc] 64:49</t>
+          <t>[DFC] 435:986</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[dfc] 75:11</t>
+          <t>[DFC] 101:851</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[dfc] 75:96</t>
+          <t>[DFC] 983:546</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[dfc] 98:12</t>
+          <t>[DFC] 368:176</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[dfc] 39:53</t>
+          <t>[DFC] 697:260</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>[dfc] 59:40</t>
+          <t>[DFC] 892:102</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>[dfc] 25:99</t>
+          <t>[DFC] 367:725</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>[dfc] 88:59</t>
+          <t>[DFC] 777:618</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>[dfc] 46:87</t>
+          <t>[DFC] 983:591</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>[dfc] 90:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="15" customHeight="1" s="7">
+          <t>[DFC] 590:284</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1" s="6">
       <c r="A23" t="inlineStr">
         <is>
-          <t>[dfc] 66:43</t>
+          <t>[DFC] 278:367</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[dfc] 31:30</t>
+          <t>[DFC] 348:403</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[dfc] 64:57</t>
+          <t>[DFC] 887:878</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[dfc] 52:54</t>
+          <t>[DFC] 962:933</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[dfc] 94:45</t>
+          <t>[DFC] 227:805</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[dfc] 84:39</t>
+          <t>[DFC] 320:603</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[dfc] 26:9</t>
+          <t>[DFC] 615:546</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>[dfc] 99:70</t>
+          <t>[DFC] 682:218</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>[dfc] 39:26</t>
+          <t>[DFC] 996:774</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>[dfc] 45:84</t>
+          <t>[DFC] 399:147</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>[dfc] 42:48</t>
+          <t>[DFC] 764:351</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>[dfc] 56:61</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" s="7">
+          <t>[DFC] 270:846</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1" s="6">
       <c r="A24" t="inlineStr">
         <is>
-          <t>[dfc] 34:14</t>
+          <t>[DFC] 505:580</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[dfc] 77:35</t>
+          <t>[DFC] 481:157</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[dfc] 27:81</t>
+          <t>[DFC] 794:182</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>[dfc] 78:87</t>
+          <t>[DFC] 254:738</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[dfc] 66:58</t>
+          <t>[DFC] 897:979</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[dfc] 83:20</t>
+          <t>[DFC] 232:634</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[dfc] 56:76</t>
+          <t>[DFC] 221:919</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>[dfc] 75:12</t>
+          <t>[DFC] 533:421</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>[dfc] 49:81</t>
+          <t>[DFC] 142:837</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>[dfc] 92:51</t>
+          <t>[DFC] 756:404</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>[dfc] 95:81</t>
+          <t>[DFC] 743:774</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>[dfc] 39:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" s="7">
+          <t>[DFC] 537:802</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1" s="6">
       <c r="A25" t="inlineStr">
         <is>
-          <t>[dfc] 45:97</t>
+          <t>[DFC] 375:720</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[dfc] 81:55</t>
+          <t>[DFC] 621:132</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[dfc] 76:43</t>
+          <t>[DFC] 893:993</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[dfc] 42:59</t>
+          <t>[DFC] 474:920</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[dfc] 55:97</t>
+          <t>[DFC] 283:386</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[dfc] 57:40</t>
+          <t>[DFC] 210:964</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[dfc] 74:30</t>
+          <t>[DFC] 844:661</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>[dfc] 75:13</t>
+          <t>[DFC] 559:912</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>[dfc] 37:22</t>
+          <t>[DFC] 854:273</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>[dfc] 71:15</t>
+          <t>[DFC] 959:412</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>[dfc] 31:64</t>
+          <t>[DFC] 122:796</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>[dfc] 57:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" s="7">
+          <t>[DFC] 620:465</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" s="6">
       <c r="A26" t="inlineStr">
         <is>
-          <t>[dfc] 96:83</t>
+          <t>[DFC] 337:984</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[dfc] 35:79</t>
+          <t>[DFC] 655:441</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[dfc] 65:52</t>
+          <t>[DFC] 288:502</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[dfc] 30:88</t>
+          <t>[DFC] 828:500</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[dfc] 57:37</t>
+          <t>[DFC] 901:166</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[dfc] 97:89</t>
+          <t>[DFC] 403:491</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[dfc] 34:57</t>
+          <t>[DFC] 101:519</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>[dfc] 99:22</t>
+          <t>[DFC] 502:332</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>[dfc] 80:65</t>
+          <t>[DFC] 384:804</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>[dfc] 68:73</t>
+          <t>[DFC] 659:469</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>[dfc] 46:47</t>
+          <t>[DFC] 757:385</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>[dfc] 65:70</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="15" customHeight="1" s="7">
+          <t>[DFC] 827:812</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" s="6">
       <c r="A27" t="inlineStr">
         <is>
-          <t>[dfc] 89:18</t>
+          <t>[DFC] 694:994</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[dfc] 49:65</t>
+          <t>[DFC] 449:963</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[dfc] 79:42</t>
+          <t>[DFC] 931:488</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[dfc] 93:65</t>
+          <t>[DFC] 140:295</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[dfc] 32:33</t>
+          <t>[DFC] 822:980</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[dfc] 54:59</t>
+          <t>[DFC] 669:998</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[dfc] 46:17</t>
+          <t>[DFC] 944:154</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>[dfc] 32:85</t>
+          <t>[DFC] 448:646</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[dfc] 71:88</t>
+          <t>[DFC] 219:225</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>[dfc] 96:30</t>
+          <t>[DFC] 166:717</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>[dfc] 48:88</t>
+          <t>[DFC] 822:475</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>[dfc] 60:83</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" s="7">
+          <t>[DFC] 571:738</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" s="6">
       <c r="A28" t="inlineStr">
         <is>
-          <t>[dfc] 32:29</t>
+          <t>[DFC] 668:689</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[dfc] 87:5</t>
+          <t>[DFC] 733:210</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[dfc] 82:51</t>
+          <t>[DFC] 453:928</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[dfc] 33:34</t>
+          <t>[DFC] 872:543</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[dfc] 72:59</t>
+          <t>[DFC] 232:741</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[dfc] 72:14</t>
+          <t>[DFC] 247:791</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[dfc] 76:54</t>
+          <t>[DFC] 500:201</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>[dfc] 78:33</t>
+          <t>[DFC] 743:948</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>[dfc] 89:79</t>
+          <t>[DFC] 588:643</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>[dfc] 33:54</t>
+          <t>[DFC] 680:517</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>[dfc] 52:30</t>
+          <t>[DFC] 373:395</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>[dfc] 42:75</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="15" customHeight="1" s="7">
+          <t>[DFC] 909:577</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1" s="6">
       <c r="A29" t="inlineStr">
         <is>
-          <t>[dfc] 92:14</t>
+          <t>[DFC] 361:334</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[dfc] 70:66</t>
+          <t>[DFC] 101:956</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[dfc] 76:82</t>
+          <t>[DFC] 951:925</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[dfc] 72:93</t>
+          <t>[DFC] 421:104</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[dfc] 57:54</t>
+          <t>[DFC] 549:430</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[dfc] 46:98</t>
+          <t>[DFC] 472:677</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[dfc] 53:14</t>
+          <t>[DFC] 630:875</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>[dfc] 30:85</t>
+          <t>[DFC] 809:221</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>[dfc] 50:98</t>
+          <t>[DFC] 292:612</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>[dfc] 50:90</t>
+          <t>[DFC] 929:187</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>[dfc] 94:48</t>
+          <t>[DFC] 599:186</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>[dfc] 96:73</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="15" customHeight="1" s="7">
+          <t>[DFC] 842:186</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1" s="6">
       <c r="A30" t="inlineStr">
         <is>
-          <t>[dfc] 48:79</t>
+          <t>[DFC] 491:569</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[dfc] 68:84</t>
+          <t>[DFC] 213:943</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[dfc] 56:78</t>
+          <t>[DFC] 849:604</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>[dfc] 91:81</t>
+          <t>[DFC] 970:938</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[dfc] 65:31</t>
+          <t>[DFC] 462:532</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[dfc] 47:91</t>
+          <t>[DFC] 719:933</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[dfc] 64:25</t>
+          <t>[DFC] 266:112</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>[dfc] 99:11</t>
+          <t>[DFC] 132:210</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>[dfc] 71:93</t>
+          <t>[DFC] 177:169</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>[dfc] 90:60</t>
+          <t>[DFC] 780:312</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>[dfc] 53:79</t>
+          <t>[DFC] 174:556</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>[dfc] 33:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="15" customHeight="1" s="7">
+          <t>[DFC] 339:825</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1" s="6">
       <c r="A31" t="inlineStr">
         <is>
-          <t>[dfc] 46:54</t>
+          <t>[DFC] 661:536</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[dfc] 43:81</t>
+          <t>[DFC] 331:746</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[dfc] 77:36</t>
+          <t>[DFC] 392:509</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[dfc] 82:79</t>
+          <t>[DFC] 950:538</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[dfc] 54:53</t>
+          <t>[DFC] 538:168</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[dfc] 40:98</t>
+          <t>[DFC] 437:904</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[dfc] 92:41</t>
+          <t>[DFC] 404:151</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>[dfc] 50:34</t>
+          <t>[DFC] 736:394</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>[dfc] 49:57</t>
+          <t>[DFC] 559:877</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>[dfc] 87:10</t>
+          <t>[DFC] 959:858</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>[dfc] 59:77</t>
+          <t>[DFC] 817:867</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>[dfc] 32:96</t>
-        </is>
-      </c>
-    </row>
-    <row r="32" ht="15" customHeight="1" s="7">
+          <t>[DFC] 108:189</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1" s="6">
       <c r="A32" t="inlineStr">
         <is>
-          <t>[dfc] 36:63</t>
+          <t>[DFC] 756:705</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[dfc] 53:40</t>
+          <t>[DFC] 653:882</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[dfc] 68:88</t>
+          <t>[DFC] 866:480</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>[dfc] 43:43</t>
+          <t>[DFC] 577:718</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[dfc] 99:45</t>
+          <t>[DFC] 752:336</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[dfc] 99:94</t>
+          <t>[DFC] 545:944</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[dfc] 90:38</t>
+          <t>[DFC] 735:757</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>[dfc] 63:12</t>
+          <t>[DFC] 716:740</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>[dfc] 85:19</t>
+          <t>[DFC] 583:575</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>[dfc] 39:24</t>
+          <t>[DFC] 323:253</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>[dfc] 95:66</t>
+          <t>[DFC] 242:750</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>[dfc] 73:21</t>
-        </is>
-      </c>
-    </row>
-    <row r="33" ht="15" customHeight="1" s="7">
+          <t>[DFC] 298:352</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1" s="6">
       <c r="A33" t="inlineStr">
         <is>
-          <t>[dfc] 45:10</t>
+          <t>[DFC] 537:742</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[dfc] 66:97</t>
+          <t>[DFC] 391:552</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[dfc] 59:26</t>
+          <t>[DFC] 743:201</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[dfc] 54:18</t>
+          <t>[DFC] 245:392</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[dfc] 49:21</t>
+          <t>[DFC] 963:947</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[dfc] 97:45</t>
+          <t>[DFC] 671:328</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[dfc] 60:86</t>
+          <t>[DFC] 583:443</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>[dfc] 66:40</t>
+          <t>[DFC] 688:681</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>[dfc] 93:54</t>
+          <t>[DFC] 291:488</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>[dfc] 92:42</t>
+          <t>[DFC] 593:444</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>[dfc] 38:33</t>
+          <t>[DFC] 853:595</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>[dfc] 68:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="15" customHeight="1" s="7">
+          <t>[DFC] 564:297</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1" s="6">
       <c r="A34" t="inlineStr">
         <is>
-          <t>[dfc] 88:48</t>
+          <t>[DFC] 571:756</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[dfc] 85:34</t>
+          <t>[DFC] 627:552</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[dfc] 74:61</t>
+          <t>[DFC] 181:927</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[dfc] 90:27</t>
+          <t>[DFC] 685:522</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[dfc] 43:86</t>
+          <t>[DFC] 392:234</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[dfc] 94:35</t>
+          <t>[DFC] 739:734</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[dfc] 60:82</t>
+          <t>[DFC] 853:392</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>[dfc] 35:28</t>
+          <t>[DFC] 458:868</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>[dfc] 89:85</t>
+          <t>[DFC] 127:598</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>[dfc] 90:64</t>
+          <t>[DFC] 306:130</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>[dfc] 45:63</t>
+          <t>[DFC] 288:753</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>[dfc] 95:35</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="15" customHeight="1" s="7">
+          <t>[DFC] 444:654</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1" s="6">
       <c r="A35" t="inlineStr">
         <is>
-          <t>[dfc] 71:9</t>
+          <t>[DFC] 123:940</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[dfc] 52:10</t>
+          <t>[DFC] 868:169</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>[dfc] 96:50</t>
+          <t>[DFC] 415:556</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[dfc] 43:84</t>
+          <t>[DFC] 200:321</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[dfc] 69:96</t>
+          <t>[DFC] 714:393</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[dfc] 80:21</t>
+          <t>[DFC] 342:647</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[dfc] 63:86</t>
+          <t>[DFC] 467:434</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>[dfc] 75:92</t>
+          <t>[DFC] 151:243</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>[dfc] 67:49</t>
+          <t>[DFC] 561:105</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>[dfc] 53:90</t>
+          <t>[DFC] 835:493</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>[dfc] 48:99</t>
+          <t>[DFC] 763:517</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>[dfc] 97:77</t>
-        </is>
-      </c>
-    </row>
-    <row r="36" ht="15" customHeight="1" s="7">
+          <t>[DFC] 588:104</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1" s="6">
       <c r="A36" t="inlineStr">
         <is>
-          <t>[dfc] 70:41</t>
+          <t>[DFC] 703:364</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[dfc] 57:23</t>
+          <t>[DFC] 579:289</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[dfc] 37:48</t>
+          <t>[DFC] 322:471</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[dfc] 44:53</t>
+          <t>[DFC] 492:836</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[dfc] 98:39</t>
+          <t>[DFC] 642:325</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[dfc] 93:96</t>
+          <t>[DFC] 700:196</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[dfc] 44:11</t>
+          <t>[DFC] 294:885</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>[dfc] 56:16</t>
+          <t>[DFC] 575:983</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>[dfc] 82:30</t>
+          <t>[DFC] 138:185</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>[dfc] 97:43</t>
+          <t>[DFC] 676:556</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>[dfc] 92:64</t>
+          <t>[DFC] 618:609</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>[dfc] 54:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="37" ht="15" customHeight="1" s="7">
+          <t>[DFC] 983:289</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1" s="6">
       <c r="A37" t="inlineStr">
         <is>
-          <t>[dfc] 96:27</t>
+          <t>[DFC] 891:122</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[dfc] 64:66</t>
+          <t>[DFC] 338:753</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[dfc] 77:93</t>
+          <t>[DFC] 317:977</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[dfc] 98:6</t>
+          <t>[DFC] 666:687</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[dfc] 67:9</t>
+          <t>[DFC] 335:954</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[dfc] 60:8</t>
+          <t>[DFC] 194:552</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[dfc] 39:8</t>
+          <t>[DFC] 968:754</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>[dfc] 51:36</t>
+          <t>[DFC] 335:448</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>[dfc] 59:70</t>
+          <t>[DFC] 410:591</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>[dfc] 71:89</t>
+          <t>[DFC] 630:402</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>[dfc] 52:71</t>
+          <t>[DFC] 370:227</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>[dfc] 44:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" ht="15" customHeight="1" s="7">
+          <t>[DFC] 352:370</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="15" customHeight="1" s="6">
       <c r="A38" t="inlineStr">
         <is>
-          <t>[dfc] 79:76</t>
+          <t>[DFC] 369:161</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[dfc] 71:67</t>
+          <t>[DFC] 185:420</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[dfc] 86:83</t>
+          <t>[DFC] 204:267</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[dfc] 86:46</t>
+          <t>[DFC] 563:648</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[dfc] 40:40</t>
+          <t>[DFC] 987:358</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[dfc] 77:37</t>
+          <t>[DFC] 588:456</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[dfc] 52:9</t>
+          <t>[DFC] 619:934</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>[dfc] 73:13</t>
+          <t>[DFC] 823:870</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[dfc] 44:89</t>
+          <t>[DFC] 561:416</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>[dfc] 60:46</t>
+          <t>[DFC] 770:575</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>[dfc] 47:20</t>
+          <t>[DFC] 523:631</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>[dfc] 73:71</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="15" customHeight="1" s="7">
+          <t>[DFC] 441:821</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1" s="6">
       <c r="A39" t="inlineStr">
         <is>
-          <t>[dfc] 48:1</t>
+          <t>[DFC] 283:268</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[dfc] 82:85</t>
+          <t>[DFC] 228:784</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[dfc] 98:47</t>
+          <t>[DFC] 816:854</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>[dfc] 67:66</t>
+          <t>[DFC] 869:736</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[dfc] 83:35</t>
+          <t>[DFC] 400:422</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[dfc] 79:17</t>
+          <t>[DFC] 246:442</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[dfc] 66:34</t>
+          <t>[DFC] 451:147</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>[dfc] 67:73</t>
+          <t>[DFC] 697:151</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>[dfc] 50:90</t>
+          <t>[DFC] 199:213</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>[dfc] 41:43</t>
+          <t>[DFC] 452:994</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>[dfc] 79:32</t>
+          <t>[DFC] 151:833</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>[dfc] 82:95</t>
-        </is>
-      </c>
-    </row>
-    <row r="40" ht="15" customHeight="1" s="7">
+          <t>[DFC] 894:469</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1" s="6">
       <c r="A40" t="inlineStr">
         <is>
-          <t>[dfc] 74:30</t>
+          <t>[DFC] 413:409</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[dfc] 43:53</t>
+          <t>[DFC] 665:341</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[dfc] 76:55</t>
+          <t>[DFC] 377:815</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[dfc] 79:85</t>
+          <t>[DFC] 506:973</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[dfc] 60:37</t>
+          <t>[DFC] 682:988</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[dfc] 92:63</t>
+          <t>[DFC] 196:534</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[dfc] 84:12</t>
+          <t>[DFC] 216:749</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>[dfc] 46:92</t>
+          <t>[DFC] 747:530</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>[dfc] 97:63</t>
+          <t>[DFC] 755:899</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>[dfc] 92:80</t>
+          <t>[DFC] 113:207</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>[dfc] 78:25</t>
+          <t>[DFC] 551:669</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>[dfc] 73:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="15" customHeight="1" s="7">
+          <t>[DFC] 109:256</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1" s="6">
       <c r="A41" t="inlineStr">
         <is>
-          <t>[dfc] 62:42</t>
+          <t>[DFC] 499:209</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[dfc] 82:38</t>
+          <t>[DFC] 167:599</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[dfc] 86:58</t>
+          <t>[DFC] 476:357</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[dfc] 94:12</t>
+          <t>[DFC] 216:711</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[dfc] 97:18</t>
+          <t>[DFC] 202:465</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[dfc] 72:17</t>
+          <t>[DFC] 776:205</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[dfc] 92:32</t>
+          <t>[DFC] 307:904</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>[dfc] 44:53</t>
+          <t>[DFC] 862:791</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>[dfc] 51:36</t>
+          <t>[DFC] 790:442</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>[dfc] 55:71</t>
+          <t>[DFC] 359:862</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>[dfc] 41:17</t>
+          <t>[DFC] 453:197</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>[dfc] 65:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="42" ht="15" customHeight="1" s="7">
+          <t>[DFC] 854:502</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" ht="15" customHeight="1" s="6">
       <c r="A42" t="inlineStr">
         <is>
-          <t>[dfc] 78:22</t>
+          <t>[DFC] 766:849</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[dfc] 51:95</t>
+          <t>[DFC] 152:877</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[dfc] 90:79</t>
+          <t>[DFC] 782:843</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>[dfc] 88:81</t>
+          <t>[DFC] 259:430</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[dfc] 76:47</t>
+          <t>[DFC] 992:907</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[dfc] 79:59</t>
+          <t>[DFC] 996:542</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[dfc] 43:91</t>
+          <t>[DFC] 608:271</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>[dfc] 91:82</t>
+          <t>[DFC] 776:304</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>[dfc] 67:9</t>
+          <t>[DFC] 773:180</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>[dfc] 80:21</t>
+          <t>[DFC] 273:812</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>[dfc] 95:63</t>
+          <t>[DFC] 590:443</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>[dfc] 56:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="43" ht="15" customHeight="1" s="7">
+          <t>[DFC] 209:854</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" ht="15" customHeight="1" s="6">
       <c r="A43" t="inlineStr">
         <is>
-          <t>[dfc] 51:26</t>
+          <t>[DFC] 853:458</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[dfc] 49:55</t>
+          <t>[DFC] 944:307</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[dfc] 84:10</t>
+          <t>[DFC] 681:391</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[dfc] 46:46</t>
+          <t>[DFC] 918:991</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[dfc] 89:22</t>
+          <t>[DFC] 918:756</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[dfc] 56:30</t>
+          <t>[DFC] 427:167</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[dfc] 82:19</t>
+          <t>[DFC] 173:525</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>[dfc] 65:63</t>
+          <t>[DFC] 314:617</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>[dfc] 44:24</t>
+          <t>[DFC] 655:542</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>[dfc] 45:51</t>
+          <t>[DFC] 299:902</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>[dfc] 45:25</t>
+          <t>[DFC] 724:841</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>[dfc] 89:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="44" ht="15" customHeight="1" s="7">
+          <t>[DFC] 709:145</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="15" customHeight="1" s="6">
       <c r="A44" t="inlineStr">
         <is>
-          <t>[dfc] 81:78</t>
+          <t>[DFC] 532:804</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[dfc] 55:3</t>
+          <t>[DFC] 280:750</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[dfc] 85:53</t>
+          <t>[DFC] 165:130</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[dfc] 85:96</t>
+          <t>[DFC] 953:288</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[dfc] 66:17</t>
+          <t>[DFC] 456:386</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[dfc] 85:22</t>
+          <t>[DFC] 386:959</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[dfc] 86:42</t>
+          <t>[DFC] 854:436</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>[dfc] 78:88</t>
+          <t>[DFC] 339:251</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[dfc] 57:61</t>
+          <t>[DFC] 649:647</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>[dfc] 91:13</t>
+          <t>[DFC] 737:708</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>[dfc] 77:55</t>
+          <t>[DFC] 141:635</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>[dfc] 87:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="45" ht="15" customHeight="1" s="7">
+          <t>[DFC] 956:316</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="15" customHeight="1" s="6">
       <c r="A45" t="inlineStr">
         <is>
-          <t>[dfc] 60:43</t>
+          <t>[DFC] 141:711</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[dfc] 97:57</t>
+          <t>[DFC] 778:211</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[dfc] 57:87</t>
+          <t>[DFC] 389:156</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[dfc] 74:36</t>
+          <t>[DFC] 152:450</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[dfc] 47:12</t>
+          <t>[DFC] 242:688</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[dfc] 88:47</t>
+          <t>[DFC] 285:722</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[dfc] 95:80</t>
+          <t>[DFC] 753:618</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>[dfc] 67:69</t>
+          <t>[DFC] 221:755</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[dfc] 49:29</t>
+          <t>[DFC] 871:170</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>[dfc] 88:26</t>
+          <t>[DFC] 100:627</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>[dfc] 69:99</t>
+          <t>[DFC] 770:622</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>[dfc] 52:99</t>
-        </is>
-      </c>
-    </row>
-    <row r="46" ht="15" customHeight="1" s="7">
+          <t>[DFC] 182:211</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" ht="15" customHeight="1" s="6">
       <c r="A46" t="inlineStr">
         <is>
-          <t>[dfc] 67:13</t>
+          <t>[DFC] 809:115</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[dfc] 78:75</t>
+          <t>[DFC] 845:675</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[dfc] 87:97</t>
+          <t>[DFC] 690:284</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[dfc] 96:76</t>
+          <t>[DFC] 612:293</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[dfc] 81:36</t>
+          <t>[DFC] 933:984</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[dfc] 46:84</t>
+          <t>[DFC] 144:476</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>[dfc] 46:49</t>
+          <t>[DFC] 621:369</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>[dfc] 86:15</t>
+          <t>[DFC] 753:107</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>[dfc] 77:14</t>
+          <t>[DFC] 254:595</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>[dfc] 56:50</t>
+          <t>[DFC] 296:524</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>[dfc] 57:72</t>
+          <t>[DFC] 483:147</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>[dfc] 65:70</t>
-        </is>
-      </c>
-    </row>
-    <row r="47" ht="15" customHeight="1" s="7">
+          <t>[DFC] 771:529</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="15" customHeight="1" s="6">
       <c r="A47" t="inlineStr">
         <is>
-          <t>[dfc] 68:81</t>
+          <t>[DFC] 390:194</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[dfc] 76:79</t>
+          <t>[DFC] 178:317</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[dfc] 79:72</t>
+          <t>[DFC] 707:505</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[dfc] 59:43</t>
+          <t>[DFC] 896:285</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[dfc] 68:40</t>
+          <t>[DFC] 120:453</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[dfc] 94:31</t>
+          <t>[DFC] 692:825</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>[dfc] 51:38</t>
+          <t>[DFC] 759:776</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>[dfc] 83:62</t>
+          <t>[DFC] 817:233</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[dfc] 56:61</t>
+          <t>[DFC] 283:132</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>[dfc] 62:83</t>
+          <t>[DFC] 771:338</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>[dfc] 87:52</t>
+          <t>[DFC] 501:125</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>[dfc] 61:88</t>
-        </is>
-      </c>
-    </row>
-    <row r="48" ht="15" customHeight="1" s="7">
+          <t>[DFC] 523:599</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="15" customHeight="1" s="6">
       <c r="A48" t="inlineStr">
         <is>
-          <t>[dfc] 62:74</t>
+          <t>[DFC] 707:921</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[dfc] 62:96</t>
+          <t>[DFC] 276:255</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[dfc] 50:55</t>
+          <t>[DFC] 226:703</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[dfc] 94:79</t>
+          <t>[DFC] 323:578</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[dfc] 71:18</t>
+          <t>[DFC] 366:393</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[dfc] 96:81</t>
+          <t>[DFC] 126:879</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>[dfc] 69:23</t>
+          <t>[DFC] 631:338</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>[dfc] 97:28</t>
+          <t>[DFC] 902:287</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>[dfc] 88:22</t>
+          <t>[DFC] 456:914</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>[dfc] 55:58</t>
+          <t>[DFC] 184:598</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>[dfc] 77:78</t>
+          <t>[DFC] 576:733</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>[dfc] 80:97</t>
-        </is>
-      </c>
-    </row>
-    <row r="49" ht="15" customHeight="1" s="7">
+          <t>[DFC] 413:289</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" ht="15" customHeight="1" s="6">
       <c r="A49" t="inlineStr">
         <is>
-          <t>[dfc] 97:19</t>
+          <t>[DFC] 716:621</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[dfc] 83:95</t>
+          <t>[DFC] 235:804</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[dfc] 62:49</t>
+          <t>[DFC] 365:495</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[dfc] 86:14</t>
+          <t>[DFC] 503:624</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[dfc] 97:50</t>
+          <t>[DFC] 333:807</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[dfc] 68:46</t>
+          <t>[DFC] 906:953</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[dfc] 83:94</t>
+          <t>[DFC] 357:646</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>[dfc] 88:98</t>
+          <t>[DFC] 887:179</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>[dfc] 70:57</t>
+          <t>[DFC] 499:800</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>[dfc] 55:49</t>
+          <t>[DFC] 468:641</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>[dfc] 83:19</t>
+          <t>[DFC] 292:144</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>[dfc] 66:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="50" ht="15" customHeight="1" s="7">
+          <t>[DFC] 532:760</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" ht="15" customHeight="1" s="6">
       <c r="A50" t="inlineStr">
         <is>
-          <t>[dfc] 85:31</t>
+          <t>[DFC] 401:487</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[dfc] 84:67</t>
+          <t>[DFC] 510:331</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[dfc] 94:88</t>
+          <t>[DFC] 350:161</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[dfc] 61:32</t>
+          <t>[DFC] 165:222</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[dfc] 71:7</t>
+          <t>[DFC] 874:424</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[dfc] 59:77</t>
+          <t>[DFC] 383:122</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[dfc] 60:77</t>
+          <t>[DFC] 207:405</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>[dfc] 69:75</t>
+          <t>[DFC] 704:249</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>[dfc] 60:51</t>
+          <t>[DFC] 389:658</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>[dfc] 85:82</t>
+          <t>[DFC] 847:877</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>[dfc] 52:26</t>
+          <t>[DFC] 586:641</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>[dfc] 99:80</t>
-        </is>
-      </c>
-    </row>
-    <row r="51" ht="15" customHeight="1" s="7"/>
-    <row r="52" ht="15" customHeight="1" s="7"/>
-    <row r="53" ht="15" customHeight="1" s="7"/>
-    <row r="54" ht="15" customHeight="1" s="7"/>
-    <row r="55" ht="15" customHeight="1" s="7"/>
-    <row r="56" ht="15" customHeight="1" s="7"/>
-    <row r="57" ht="15" customHeight="1" s="7"/>
-    <row r="58" ht="15" customHeight="1" s="7"/>
-    <row r="59" ht="15" customHeight="1" s="7"/>
-    <row r="60" ht="15" customHeight="1" s="7"/>
-    <row r="61" ht="15" customHeight="1" s="7"/>
-    <row r="62" ht="15" customHeight="1" s="7"/>
-    <row r="63" ht="15" customHeight="1" s="7"/>
-    <row r="64" ht="15" customHeight="1" s="7"/>
-    <row r="65" ht="15" customHeight="1" s="7"/>
-    <row r="66" ht="15" customHeight="1" s="7"/>
-    <row r="67" ht="15" customHeight="1" s="7"/>
-    <row r="68" ht="15" customHeight="1" s="7"/>
-    <row r="69" ht="15" customHeight="1" s="7"/>
-    <row r="70" ht="15" customHeight="1" s="7"/>
-    <row r="71" ht="15" customHeight="1" s="7"/>
-    <row r="72" ht="15" customHeight="1" s="7"/>
-    <row r="73" ht="15" customHeight="1" s="7"/>
-    <row r="74" ht="15" customHeight="1" s="7"/>
-    <row r="75" ht="15" customHeight="1" s="7"/>
-    <row r="76" ht="15" customHeight="1" s="7"/>
-    <row r="77" ht="15" customHeight="1" s="7"/>
-    <row r="78" ht="15" customHeight="1" s="7"/>
-    <row r="79" ht="15" customHeight="1" s="7"/>
-    <row r="80" ht="15" customHeight="1" s="7"/>
-    <row r="81" ht="15" customHeight="1" s="7"/>
-    <row r="82" ht="15" customHeight="1" s="7"/>
-    <row r="83" ht="15" customHeight="1" s="7"/>
-    <row r="84" ht="15" customHeight="1" s="7"/>
-    <row r="85" ht="15" customHeight="1" s="7"/>
-    <row r="86" ht="15" customHeight="1" s="7"/>
-    <row r="87" ht="15" customHeight="1" s="7"/>
-    <row r="88" ht="15" customHeight="1" s="7"/>
-    <row r="89" ht="15" customHeight="1" s="7"/>
-    <row r="90" ht="15" customHeight="1" s="7"/>
-    <row r="91" ht="15" customHeight="1" s="7"/>
-    <row r="92" ht="15" customHeight="1" s="7"/>
-    <row r="93" ht="15" customHeight="1" s="7"/>
-    <row r="94" ht="15" customHeight="1" s="7"/>
-    <row r="95" ht="15" customHeight="1" s="7"/>
-    <row r="96" ht="15" customHeight="1" s="7"/>
-    <row r="97" ht="15" customHeight="1" s="7"/>
-    <row r="98" ht="15" customHeight="1" s="7"/>
-    <row r="99" ht="15" customHeight="1" s="7"/>
-    <row r="100" ht="15" customHeight="1" s="7"/>
-    <row r="101" ht="15" customHeight="1" s="7"/>
-    <row r="102" ht="15" customHeight="1" s="7"/>
-    <row r="103" ht="15" customHeight="1" s="7"/>
-    <row r="104" ht="15" customHeight="1" s="7"/>
-    <row r="105" ht="15" customHeight="1" s="7"/>
-    <row r="106" ht="15" customHeight="1" s="7"/>
-    <row r="107" ht="15" customHeight="1" s="7"/>
-    <row r="108" ht="15" customHeight="1" s="7"/>
-    <row r="109" ht="15" customHeight="1" s="7"/>
-    <row r="110" ht="15" customHeight="1" s="7"/>
-    <row r="111" ht="15" customHeight="1" s="7"/>
-    <row r="112" ht="15" customHeight="1" s="7"/>
-    <row r="113" ht="15" customHeight="1" s="7"/>
-    <row r="114" ht="15" customHeight="1" s="7"/>
-    <row r="115" ht="15" customHeight="1" s="7"/>
-    <row r="116" ht="15" customHeight="1" s="7"/>
-    <row r="117" ht="15" customHeight="1" s="7"/>
-    <row r="118" ht="15" customHeight="1" s="7"/>
-    <row r="119" ht="15" customHeight="1" s="7"/>
-    <row r="120" ht="15" customHeight="1" s="7"/>
-    <row r="121" ht="15" customHeight="1" s="7"/>
-    <row r="122" ht="15" customHeight="1" s="7"/>
-    <row r="123" ht="15" customHeight="1" s="7"/>
-    <row r="124" ht="15" customHeight="1" s="7"/>
-    <row r="125" ht="15" customHeight="1" s="7"/>
-    <row r="126" ht="15" customHeight="1" s="7"/>
-    <row r="127" ht="15" customHeight="1" s="7"/>
-    <row r="128" ht="15" customHeight="1" s="7"/>
-    <row r="129" ht="15" customHeight="1" s="7"/>
-    <row r="130" ht="15" customHeight="1" s="7"/>
-    <row r="131" ht="15" customHeight="1" s="7"/>
-    <row r="132" ht="15" customHeight="1" s="7"/>
-    <row r="133" ht="15" customHeight="1" s="7"/>
-    <row r="134" ht="15" customHeight="1" s="7"/>
-    <row r="135" ht="15" customHeight="1" s="7"/>
-    <row r="136" ht="15" customHeight="1" s="7"/>
-    <row r="137" ht="15" customHeight="1" s="7"/>
-    <row r="138" ht="15" customHeight="1" s="7"/>
-    <row r="139" ht="15" customHeight="1" s="7"/>
-    <row r="140" ht="15" customHeight="1" s="7"/>
-    <row r="141" ht="15" customHeight="1" s="7"/>
-    <row r="142" ht="15" customHeight="1" s="7"/>
-    <row r="143" ht="15" customHeight="1" s="7"/>
-    <row r="144" ht="15" customHeight="1" s="7"/>
-    <row r="145" ht="15" customHeight="1" s="7"/>
-    <row r="146" ht="15" customHeight="1" s="7"/>
-    <row r="147" ht="15" customHeight="1" s="7"/>
-    <row r="148" ht="15" customHeight="1" s="7"/>
-    <row r="149" ht="15" customHeight="1" s="7"/>
-    <row r="150" ht="15" customHeight="1" s="7"/>
-    <row r="151" ht="15" customHeight="1" s="7"/>
-    <row r="152" ht="15" customHeight="1" s="7"/>
-    <row r="153" ht="15" customHeight="1" s="7"/>
-    <row r="154" ht="15" customHeight="1" s="7"/>
-    <row r="155" ht="15" customHeight="1" s="7"/>
-    <row r="156" ht="15" customHeight="1" s="7"/>
-    <row r="157" ht="15" customHeight="1" s="7"/>
-    <row r="158" ht="15" customHeight="1" s="7"/>
-    <row r="159" ht="15" customHeight="1" s="7"/>
-    <row r="160" ht="15" customHeight="1" s="7"/>
-    <row r="161" ht="15" customHeight="1" s="7"/>
-    <row r="162" ht="15" customHeight="1" s="7"/>
-    <row r="163" ht="15" customHeight="1" s="7"/>
-    <row r="164" ht="15" customHeight="1" s="7"/>
-    <row r="165" ht="15" customHeight="1" s="7"/>
-    <row r="166" ht="15" customHeight="1" s="7"/>
-    <row r="167" ht="15" customHeight="1" s="7"/>
-    <row r="168" ht="15" customHeight="1" s="7"/>
-    <row r="169" ht="15" customHeight="1" s="7"/>
-    <row r="170" ht="15" customHeight="1" s="7"/>
-    <row r="171" ht="15" customHeight="1" s="7"/>
-    <row r="172" ht="15" customHeight="1" s="7"/>
-    <row r="173" ht="15" customHeight="1" s="7"/>
-    <row r="174" ht="15" customHeight="1" s="7"/>
-    <row r="175" ht="15" customHeight="1" s="7"/>
-    <row r="176" ht="15" customHeight="1" s="7"/>
-    <row r="177" ht="15" customHeight="1" s="7"/>
-    <row r="178" ht="15" customHeight="1" s="7"/>
-    <row r="179" ht="15" customHeight="1" s="7"/>
-    <row r="180" ht="15" customHeight="1" s="7"/>
-    <row r="181" ht="15" customHeight="1" s="7"/>
-    <row r="182" ht="15" customHeight="1" s="7"/>
-    <row r="183" ht="15" customHeight="1" s="7"/>
-    <row r="184" ht="15" customHeight="1" s="7"/>
-    <row r="185" ht="15" customHeight="1" s="7"/>
-    <row r="186" ht="15" customHeight="1" s="7"/>
-    <row r="187" ht="15" customHeight="1" s="7"/>
-    <row r="188" ht="15" customHeight="1" s="7"/>
-    <row r="189" ht="15" customHeight="1" s="7"/>
-    <row r="190" ht="15" customHeight="1" s="7"/>
-    <row r="191" ht="15" customHeight="1" s="7"/>
-    <row r="192" ht="15" customHeight="1" s="7"/>
-    <row r="193" ht="15" customHeight="1" s="7"/>
-    <row r="194" ht="15" customHeight="1" s="7"/>
-    <row r="195" ht="15" customHeight="1" s="7"/>
-    <row r="196" ht="15" customHeight="1" s="7"/>
-    <row r="197" ht="15" customHeight="1" s="7"/>
-    <row r="198" ht="15" customHeight="1" s="7"/>
-    <row r="199" ht="15" customHeight="1" s="7"/>
-    <row r="200" ht="15" customHeight="1" s="7"/>
-    <row r="201" ht="15" customHeight="1" s="7"/>
-    <row r="202" ht="15" customHeight="1" s="7"/>
-    <row r="203" ht="15" customHeight="1" s="7"/>
-    <row r="204" ht="15" customHeight="1" s="7"/>
-    <row r="205" ht="15" customHeight="1" s="7"/>
-    <row r="206" ht="15" customHeight="1" s="7"/>
-    <row r="207" ht="15" customHeight="1" s="7"/>
-    <row r="208" ht="15" customHeight="1" s="7"/>
-    <row r="209" ht="15" customHeight="1" s="7"/>
-    <row r="210" ht="15" customHeight="1" s="7"/>
-    <row r="211" ht="15" customHeight="1" s="7"/>
-    <row r="212" ht="15" customHeight="1" s="7"/>
-    <row r="213" ht="15" customHeight="1" s="7"/>
-    <row r="214" ht="15" customHeight="1" s="7"/>
-    <row r="215" ht="15" customHeight="1" s="7"/>
-    <row r="216" ht="15" customHeight="1" s="7"/>
-    <row r="217" ht="15" customHeight="1" s="7"/>
-    <row r="218" ht="15" customHeight="1" s="7"/>
-    <row r="219" ht="15" customHeight="1" s="7"/>
-    <row r="220" ht="15" customHeight="1" s="7"/>
-    <row r="221" ht="15" customHeight="1" s="7"/>
-    <row r="222" ht="15" customHeight="1" s="7"/>
-    <row r="223" ht="15" customHeight="1" s="7"/>
-    <row r="224" ht="15" customHeight="1" s="7"/>
-    <row r="225" ht="15" customHeight="1" s="7"/>
-    <row r="226" ht="15" customHeight="1" s="7"/>
-    <row r="227" ht="15" customHeight="1" s="7"/>
-    <row r="228" ht="15" customHeight="1" s="7"/>
-    <row r="229" ht="15" customHeight="1" s="7"/>
-    <row r="230" ht="15" customHeight="1" s="7"/>
-    <row r="231" ht="15" customHeight="1" s="7"/>
-    <row r="232" ht="15" customHeight="1" s="7"/>
-    <row r="233" ht="15" customHeight="1" s="7"/>
-    <row r="234" ht="15" customHeight="1" s="7"/>
-    <row r="235" ht="15" customHeight="1" s="7"/>
-    <row r="236" ht="15" customHeight="1" s="7"/>
-    <row r="237" ht="15" customHeight="1" s="7"/>
-    <row r="238" ht="15" customHeight="1" s="7"/>
-    <row r="239" ht="15" customHeight="1" s="7"/>
-    <row r="240" ht="15" customHeight="1" s="7"/>
-    <row r="241" ht="15" customHeight="1" s="7"/>
-    <row r="242" ht="15" customHeight="1" s="7"/>
-    <row r="243" ht="15" customHeight="1" s="7"/>
-    <row r="244" ht="15" customHeight="1" s="7"/>
-    <row r="245" ht="15" customHeight="1" s="7"/>
-    <row r="246" ht="15" customHeight="1" s="7"/>
-    <row r="247" ht="15" customHeight="1" s="7"/>
-    <row r="248" ht="15" customHeight="1" s="7"/>
-    <row r="249" ht="15" customHeight="1" s="7"/>
-    <row r="250" ht="15" customHeight="1" s="7"/>
-    <row r="251" ht="15" customHeight="1" s="7"/>
-    <row r="252" ht="15" customHeight="1" s="7"/>
-    <row r="253" ht="15" customHeight="1" s="7"/>
-    <row r="254" ht="15" customHeight="1" s="7"/>
-    <row r="255" ht="15" customHeight="1" s="7"/>
-    <row r="256" ht="15" customHeight="1" s="7"/>
-    <row r="257" ht="15" customHeight="1" s="7"/>
-    <row r="258" ht="15" customHeight="1" s="7"/>
-    <row r="259" ht="15" customHeight="1" s="7"/>
-    <row r="260" ht="15" customHeight="1" s="7"/>
-    <row r="261" ht="15" customHeight="1" s="7"/>
-    <row r="262" ht="15" customHeight="1" s="7"/>
-    <row r="263" ht="15" customHeight="1" s="7"/>
-    <row r="264" ht="15" customHeight="1" s="7"/>
-    <row r="265" ht="15" customHeight="1" s="7"/>
-    <row r="266" ht="15" customHeight="1" s="7"/>
-    <row r="267" ht="15" customHeight="1" s="7"/>
-    <row r="268" ht="15" customHeight="1" s="7"/>
-    <row r="269" ht="15" customHeight="1" s="7"/>
-    <row r="270" ht="15" customHeight="1" s="7"/>
-    <row r="271" ht="15" customHeight="1" s="7"/>
-    <row r="272" ht="15" customHeight="1" s="7"/>
-    <row r="273" ht="15" customHeight="1" s="7"/>
-    <row r="274" ht="15" customHeight="1" s="7"/>
-    <row r="275" ht="15" customHeight="1" s="7"/>
-    <row r="276" ht="15" customHeight="1" s="7"/>
-    <row r="277" ht="15" customHeight="1" s="7"/>
-    <row r="278" ht="15" customHeight="1" s="7"/>
-    <row r="279" ht="15" customHeight="1" s="7"/>
-    <row r="280" ht="15" customHeight="1" s="7"/>
-    <row r="281" ht="15" customHeight="1" s="7"/>
-    <row r="282" ht="15" customHeight="1" s="7"/>
-    <row r="283" ht="15" customHeight="1" s="7"/>
-    <row r="284" ht="15" customHeight="1" s="7"/>
-    <row r="285" ht="15" customHeight="1" s="7"/>
-    <row r="286" ht="15" customHeight="1" s="7"/>
-    <row r="287" ht="15" customHeight="1" s="7"/>
-    <row r="288" ht="15" customHeight="1" s="7"/>
-    <row r="289" ht="15" customHeight="1" s="7"/>
-    <row r="290" ht="15" customHeight="1" s="7"/>
-    <row r="291" ht="15" customHeight="1" s="7"/>
-    <row r="292" ht="15" customHeight="1" s="7"/>
-    <row r="293" ht="15" customHeight="1" s="7"/>
-    <row r="294" ht="15" customHeight="1" s="7"/>
-    <row r="295" ht="15" customHeight="1" s="7"/>
-    <row r="296" ht="15" customHeight="1" s="7"/>
-    <row r="297" ht="15" customHeight="1" s="7"/>
-    <row r="298" ht="15" customHeight="1" s="7"/>
-    <row r="299" ht="15" customHeight="1" s="7"/>
-    <row r="300" ht="15" customHeight="1" s="7"/>
-    <row r="301" ht="15" customHeight="1" s="7"/>
-    <row r="302" ht="15" customHeight="1" s="7"/>
-    <row r="303" ht="15" customHeight="1" s="7"/>
-    <row r="304" ht="15" customHeight="1" s="7"/>
-    <row r="305" ht="15" customHeight="1" s="7"/>
-    <row r="306" ht="15" customHeight="1" s="7"/>
-    <row r="307" ht="15" customHeight="1" s="7"/>
-    <row r="308" ht="15" customHeight="1" s="7"/>
-    <row r="309" ht="15" customHeight="1" s="7"/>
-    <row r="310" ht="15" customHeight="1" s="7"/>
-    <row r="311" ht="15" customHeight="1" s="7"/>
-    <row r="312" ht="15" customHeight="1" s="7"/>
-    <row r="313" ht="15" customHeight="1" s="7"/>
-    <row r="314" ht="15" customHeight="1" s="7"/>
-    <row r="315" ht="15" customHeight="1" s="7"/>
-    <row r="316" ht="15" customHeight="1" s="7"/>
-    <row r="317" ht="15" customHeight="1" s="7"/>
-    <row r="318" ht="15" customHeight="1" s="7"/>
-    <row r="319" ht="15" customHeight="1" s="7"/>
-    <row r="320" ht="15" customHeight="1" s="7"/>
-    <row r="321" ht="15" customHeight="1" s="7"/>
-    <row r="322" ht="15" customHeight="1" s="7"/>
-    <row r="323" ht="15" customHeight="1" s="7"/>
-    <row r="324" ht="15" customHeight="1" s="7"/>
-    <row r="325" ht="15" customHeight="1" s="7"/>
-    <row r="326" ht="15" customHeight="1" s="7"/>
-    <row r="327" ht="15" customHeight="1" s="7"/>
-    <row r="328" ht="15" customHeight="1" s="7"/>
-    <row r="329" ht="15" customHeight="1" s="7"/>
-    <row r="330" ht="15" customHeight="1" s="7"/>
-    <row r="331" ht="15" customHeight="1" s="7"/>
-    <row r="332" ht="15" customHeight="1" s="7"/>
-    <row r="333" ht="15" customHeight="1" s="7"/>
-    <row r="334" ht="15" customHeight="1" s="7"/>
-    <row r="335" ht="15" customHeight="1" s="7"/>
-    <row r="336" ht="15" customHeight="1" s="7"/>
-    <row r="337" ht="15" customHeight="1" s="7"/>
-    <row r="338" ht="15" customHeight="1" s="7"/>
-    <row r="339" ht="15" customHeight="1" s="7"/>
-    <row r="340" ht="15" customHeight="1" s="7"/>
-    <row r="341" ht="15" customHeight="1" s="7"/>
-    <row r="342" ht="15" customHeight="1" s="7"/>
-    <row r="343" ht="15" customHeight="1" s="7"/>
-    <row r="344" ht="15" customHeight="1" s="7"/>
-    <row r="345" ht="15" customHeight="1" s="7"/>
-    <row r="346" ht="15" customHeight="1" s="7"/>
-    <row r="347" ht="15" customHeight="1" s="7"/>
-    <row r="348" ht="15" customHeight="1" s="7"/>
-    <row r="349" ht="15" customHeight="1" s="7"/>
-    <row r="350" ht="15" customHeight="1" s="7"/>
-    <row r="351" ht="15" customHeight="1" s="7"/>
-    <row r="352" ht="15" customHeight="1" s="7"/>
-    <row r="353" ht="15" customHeight="1" s="7"/>
-    <row r="354" ht="15" customHeight="1" s="7"/>
-    <row r="355" ht="15" customHeight="1" s="7"/>
-    <row r="356" ht="15" customHeight="1" s="7"/>
-    <row r="357" ht="15" customHeight="1" s="7"/>
-    <row r="358" ht="15" customHeight="1" s="7"/>
-    <row r="359" ht="15" customHeight="1" s="7"/>
-    <row r="360" ht="15" customHeight="1" s="7"/>
-    <row r="361" ht="15" customHeight="1" s="7"/>
-    <row r="362" ht="15" customHeight="1" s="7"/>
-    <row r="363" ht="15" customHeight="1" s="7"/>
-    <row r="364" ht="15" customHeight="1" s="7"/>
-    <row r="365" ht="15" customHeight="1" s="7"/>
-    <row r="366" ht="15" customHeight="1" s="7"/>
-    <row r="367" ht="15" customHeight="1" s="7"/>
-    <row r="368" ht="15" customHeight="1" s="7"/>
-    <row r="369" ht="15" customHeight="1" s="7"/>
-    <row r="370" ht="15" customHeight="1" s="7"/>
-    <row r="371" ht="15" customHeight="1" s="7"/>
-    <row r="372" ht="15" customHeight="1" s="7"/>
-    <row r="373" ht="15" customHeight="1" s="7"/>
-    <row r="374" ht="15" customHeight="1" s="7"/>
-    <row r="375" ht="15" customHeight="1" s="7"/>
-    <row r="376" ht="15" customHeight="1" s="7"/>
-    <row r="377" ht="15" customHeight="1" s="7"/>
-    <row r="378" ht="15" customHeight="1" s="7"/>
-    <row r="379" ht="15" customHeight="1" s="7"/>
-    <row r="380" ht="15" customHeight="1" s="7"/>
-    <row r="381" ht="15" customHeight="1" s="7"/>
-    <row r="382" ht="15" customHeight="1" s="7"/>
-    <row r="383" ht="15" customHeight="1" s="7"/>
-    <row r="384" ht="15" customHeight="1" s="7"/>
-    <row r="385" ht="15" customHeight="1" s="7"/>
-    <row r="386" ht="15" customHeight="1" s="7"/>
-    <row r="387" ht="15" customHeight="1" s="7"/>
-    <row r="388" ht="15" customHeight="1" s="7"/>
-    <row r="389" ht="15" customHeight="1" s="7"/>
-    <row r="390" ht="15" customHeight="1" s="7"/>
-    <row r="391" ht="15" customHeight="1" s="7"/>
-    <row r="392" ht="15" customHeight="1" s="7"/>
-    <row r="393" ht="15" customHeight="1" s="7"/>
-    <row r="394" ht="15" customHeight="1" s="7"/>
-    <row r="395" ht="15" customHeight="1" s="7"/>
-    <row r="396" ht="15" customHeight="1" s="7"/>
-    <row r="397" ht="15" customHeight="1" s="7"/>
-    <row r="398" ht="15" customHeight="1" s="7"/>
-    <row r="399" ht="15" customHeight="1" s="7"/>
-    <row r="400" ht="15" customHeight="1" s="7"/>
-    <row r="401" ht="15" customHeight="1" s="7"/>
-    <row r="402" ht="15" customHeight="1" s="7"/>
-    <row r="403" ht="15" customHeight="1" s="7"/>
-    <row r="404" ht="15" customHeight="1" s="7"/>
-    <row r="405" ht="15" customHeight="1" s="7"/>
-    <row r="406" ht="15" customHeight="1" s="7"/>
-    <row r="407" ht="15" customHeight="1" s="7"/>
-    <row r="408" ht="15" customHeight="1" s="7"/>
-    <row r="409" ht="15" customHeight="1" s="7"/>
-    <row r="410" ht="15" customHeight="1" s="7"/>
-    <row r="411" ht="15" customHeight="1" s="7"/>
-    <row r="412" ht="15" customHeight="1" s="7"/>
-    <row r="413" ht="15" customHeight="1" s="7"/>
-    <row r="414" ht="15" customHeight="1" s="7"/>
-    <row r="415" ht="15" customHeight="1" s="7"/>
-    <row r="416" ht="15" customHeight="1" s="7"/>
-    <row r="417" ht="15" customHeight="1" s="7"/>
-    <row r="418" ht="15" customHeight="1" s="7"/>
-    <row r="419" ht="15" customHeight="1" s="7"/>
-    <row r="420" ht="15" customHeight="1" s="7"/>
-    <row r="421" ht="15" customHeight="1" s="7"/>
-    <row r="422" ht="15" customHeight="1" s="7"/>
-    <row r="423" ht="15" customHeight="1" s="7"/>
-    <row r="424" ht="15" customHeight="1" s="7"/>
-    <row r="425" ht="15" customHeight="1" s="7"/>
-    <row r="426" ht="15" customHeight="1" s="7"/>
-    <row r="427" ht="15" customHeight="1" s="7"/>
-    <row r="428" ht="15" customHeight="1" s="7"/>
-    <row r="429" ht="15" customHeight="1" s="7"/>
-    <row r="430" ht="15" customHeight="1" s="7"/>
-    <row r="431" ht="15" customHeight="1" s="7"/>
-    <row r="432" ht="15" customHeight="1" s="7"/>
-    <row r="433" ht="15" customHeight="1" s="7"/>
-    <row r="434" ht="15" customHeight="1" s="7"/>
-    <row r="435" ht="15" customHeight="1" s="7"/>
-    <row r="436" ht="15" customHeight="1" s="7"/>
-    <row r="437" ht="15" customHeight="1" s="7"/>
-    <row r="438" ht="15" customHeight="1" s="7"/>
-    <row r="439" ht="15" customHeight="1" s="7"/>
-    <row r="440" ht="15" customHeight="1" s="7"/>
-    <row r="441" ht="15" customHeight="1" s="7"/>
-    <row r="442" ht="15" customHeight="1" s="7"/>
-    <row r="443" ht="15" customHeight="1" s="7"/>
-    <row r="444" ht="15" customHeight="1" s="7"/>
-    <row r="445" ht="15" customHeight="1" s="7"/>
-    <row r="446" ht="15" customHeight="1" s="7"/>
-    <row r="447" ht="15" customHeight="1" s="7"/>
-    <row r="448" ht="15" customHeight="1" s="7"/>
-    <row r="449" ht="15" customHeight="1" s="7"/>
-    <row r="450" ht="15" customHeight="1" s="7"/>
-    <row r="451" ht="15" customHeight="1" s="7"/>
-    <row r="452" ht="15" customHeight="1" s="7"/>
-    <row r="453" ht="15" customHeight="1" s="7"/>
-    <row r="454" ht="15" customHeight="1" s="7"/>
-    <row r="455" ht="15" customHeight="1" s="7"/>
-    <row r="456" ht="15" customHeight="1" s="7"/>
-    <row r="457" ht="15" customHeight="1" s="7"/>
-    <row r="458" ht="15" customHeight="1" s="7"/>
-    <row r="459" ht="15" customHeight="1" s="7"/>
-    <row r="460" ht="15" customHeight="1" s="7"/>
-    <row r="461" ht="15" customHeight="1" s="7"/>
-    <row r="462" ht="15" customHeight="1" s="7"/>
-    <row r="463" ht="15" customHeight="1" s="7"/>
-    <row r="464" ht="15" customHeight="1" s="7"/>
-    <row r="465" ht="15" customHeight="1" s="7"/>
-    <row r="466" ht="15" customHeight="1" s="7"/>
-    <row r="467" ht="15" customHeight="1" s="7"/>
-    <row r="468" ht="15" customHeight="1" s="7"/>
-    <row r="469" ht="15" customHeight="1" s="7"/>
-    <row r="470" ht="15" customHeight="1" s="7"/>
-    <row r="471" ht="15" customHeight="1" s="7"/>
-    <row r="472" ht="15" customHeight="1" s="7"/>
-    <row r="473" ht="15" customHeight="1" s="7"/>
-    <row r="474" ht="15" customHeight="1" s="7"/>
-    <row r="475" ht="15" customHeight="1" s="7"/>
-    <row r="476" ht="15" customHeight="1" s="7"/>
-    <row r="477" ht="15" customHeight="1" s="7"/>
-    <row r="478" ht="15" customHeight="1" s="7"/>
-    <row r="479" ht="15" customHeight="1" s="7"/>
-    <row r="480" ht="15" customHeight="1" s="7"/>
-    <row r="481" ht="15" customHeight="1" s="7"/>
-    <row r="482" ht="15" customHeight="1" s="7"/>
-    <row r="483" ht="15" customHeight="1" s="7"/>
-    <row r="484" ht="15" customHeight="1" s="7"/>
-    <row r="485" ht="15" customHeight="1" s="7"/>
-    <row r="486" ht="15" customHeight="1" s="7"/>
-    <row r="487" ht="15" customHeight="1" s="7"/>
-    <row r="488" ht="15" customHeight="1" s="7"/>
-    <row r="489" ht="15" customHeight="1" s="7"/>
-    <row r="490" ht="15" customHeight="1" s="7"/>
-    <row r="491" ht="15" customHeight="1" s="7"/>
-    <row r="492" ht="15" customHeight="1" s="7"/>
-    <row r="493" ht="15" customHeight="1" s="7"/>
-    <row r="494" ht="15" customHeight="1" s="7"/>
-    <row r="495" ht="15" customHeight="1" s="7"/>
-    <row r="496" ht="15" customHeight="1" s="7"/>
-    <row r="497" ht="15" customHeight="1" s="7"/>
-    <row r="498" ht="15" customHeight="1" s="7"/>
-    <row r="499" ht="15" customHeight="1" s="7"/>
-    <row r="500" ht="15" customHeight="1" s="7"/>
+          <t>[DFC] 911:744</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" ht="15" customHeight="1" s="6"/>
+    <row r="52" ht="15" customHeight="1" s="6"/>
+    <row r="53" ht="15" customHeight="1" s="6"/>
+    <row r="54" ht="15" customHeight="1" s="6"/>
+    <row r="55" ht="15" customHeight="1" s="6"/>
+    <row r="56" ht="15" customHeight="1" s="6"/>
+    <row r="57" ht="15" customHeight="1" s="6"/>
+    <row r="58" ht="15" customHeight="1" s="6"/>
+    <row r="59" ht="15" customHeight="1" s="6"/>
+    <row r="60" ht="15" customHeight="1" s="6"/>
+    <row r="61" ht="15" customHeight="1" s="6"/>
+    <row r="62" ht="15" customHeight="1" s="6"/>
+    <row r="63" ht="15" customHeight="1" s="6"/>
+    <row r="64" ht="15" customHeight="1" s="6"/>
+    <row r="65" ht="15" customHeight="1" s="6"/>
+    <row r="66" ht="15" customHeight="1" s="6"/>
+    <row r="67" ht="15" customHeight="1" s="6"/>
+    <row r="68" ht="15" customHeight="1" s="6"/>
+    <row r="69" ht="15" customHeight="1" s="6"/>
+    <row r="70" ht="15" customHeight="1" s="6"/>
+    <row r="71" ht="15" customHeight="1" s="6"/>
+    <row r="72" ht="15" customHeight="1" s="6"/>
+    <row r="73" ht="15" customHeight="1" s="6"/>
+    <row r="74" ht="15" customHeight="1" s="6"/>
+    <row r="75" ht="15" customHeight="1" s="6"/>
+    <row r="76" ht="15" customHeight="1" s="6"/>
+    <row r="77" ht="15" customHeight="1" s="6"/>
+    <row r="78" ht="15" customHeight="1" s="6"/>
+    <row r="79" ht="15" customHeight="1" s="6"/>
+    <row r="80" ht="15" customHeight="1" s="6"/>
+    <row r="81" ht="15" customHeight="1" s="6"/>
+    <row r="82" ht="15" customHeight="1" s="6"/>
+    <row r="83" ht="15" customHeight="1" s="6"/>
+    <row r="84" ht="15" customHeight="1" s="6"/>
+    <row r="85" ht="15" customHeight="1" s="6"/>
+    <row r="86" ht="15" customHeight="1" s="6"/>
+    <row r="87" ht="15" customHeight="1" s="6"/>
+    <row r="88" ht="15" customHeight="1" s="6"/>
+    <row r="89" ht="15" customHeight="1" s="6"/>
+    <row r="90" ht="15" customHeight="1" s="6"/>
+    <row r="91" ht="15" customHeight="1" s="6"/>
+    <row r="92" ht="15" customHeight="1" s="6"/>
+    <row r="93" ht="15" customHeight="1" s="6"/>
+    <row r="94" ht="15" customHeight="1" s="6"/>
+    <row r="95" ht="15" customHeight="1" s="6"/>
+    <row r="96" ht="15" customHeight="1" s="6"/>
+    <row r="97" ht="15" customHeight="1" s="6"/>
+    <row r="98" ht="15" customHeight="1" s="6"/>
+    <row r="99" ht="15" customHeight="1" s="6"/>
+    <row r="100" ht="15" customHeight="1" s="6"/>
+    <row r="101" ht="15" customHeight="1" s="6"/>
+    <row r="102" ht="15" customHeight="1" s="6"/>
+    <row r="103" ht="15" customHeight="1" s="6"/>
+    <row r="104" ht="15" customHeight="1" s="6"/>
+    <row r="105" ht="15" customHeight="1" s="6"/>
+    <row r="106" ht="15" customHeight="1" s="6"/>
+    <row r="107" ht="15" customHeight="1" s="6"/>
+    <row r="108" ht="15" customHeight="1" s="6"/>
+    <row r="109" ht="15" customHeight="1" s="6"/>
+    <row r="110" ht="15" customHeight="1" s="6"/>
+    <row r="111" ht="15" customHeight="1" s="6"/>
+    <row r="112" ht="15" customHeight="1" s="6"/>
+    <row r="113" ht="15" customHeight="1" s="6"/>
+    <row r="114" ht="15" customHeight="1" s="6"/>
+    <row r="115" ht="15" customHeight="1" s="6"/>
+    <row r="116" ht="15" customHeight="1" s="6"/>
+    <row r="117" ht="15" customHeight="1" s="6"/>
+    <row r="118" ht="15" customHeight="1" s="6"/>
+    <row r="119" ht="15" customHeight="1" s="6"/>
+    <row r="120" ht="15" customHeight="1" s="6"/>
+    <row r="121" ht="15" customHeight="1" s="6"/>
+    <row r="122" ht="15" customHeight="1" s="6"/>
+    <row r="123" ht="15" customHeight="1" s="6"/>
+    <row r="124" ht="15" customHeight="1" s="6"/>
+    <row r="125" ht="15" customHeight="1" s="6"/>
+    <row r="126" ht="15" customHeight="1" s="6"/>
+    <row r="127" ht="15" customHeight="1" s="6"/>
+    <row r="128" ht="15" customHeight="1" s="6"/>
+    <row r="129" ht="15" customHeight="1" s="6"/>
+    <row r="130" ht="15" customHeight="1" s="6"/>
+    <row r="131" ht="15" customHeight="1" s="6"/>
+    <row r="132" ht="15" customHeight="1" s="6"/>
+    <row r="133" ht="15" customHeight="1" s="6"/>
+    <row r="134" ht="15" customHeight="1" s="6"/>
+    <row r="135" ht="15" customHeight="1" s="6"/>
+    <row r="136" ht="15" customHeight="1" s="6"/>
+    <row r="137" ht="15" customHeight="1" s="6"/>
+    <row r="138" ht="15" customHeight="1" s="6"/>
+    <row r="139" ht="15" customHeight="1" s="6"/>
+    <row r="140" ht="15" customHeight="1" s="6"/>
+    <row r="141" ht="15" customHeight="1" s="6"/>
+    <row r="142" ht="15" customHeight="1" s="6"/>
+    <row r="143" ht="15" customHeight="1" s="6"/>
+    <row r="144" ht="15" customHeight="1" s="6"/>
+    <row r="145" ht="15" customHeight="1" s="6"/>
+    <row r="146" ht="15" customHeight="1" s="6"/>
+    <row r="147" ht="15" customHeight="1" s="6"/>
+    <row r="148" ht="15" customHeight="1" s="6"/>
+    <row r="149" ht="15" customHeight="1" s="6"/>
+    <row r="150" ht="15" customHeight="1" s="6"/>
+    <row r="151" ht="15" customHeight="1" s="6"/>
+    <row r="152" ht="15" customHeight="1" s="6"/>
+    <row r="153" ht="15" customHeight="1" s="6"/>
+    <row r="154" ht="15" customHeight="1" s="6"/>
+    <row r="155" ht="15" customHeight="1" s="6"/>
+    <row r="156" ht="15" customHeight="1" s="6"/>
+    <row r="157" ht="15" customHeight="1" s="6"/>
+    <row r="158" ht="15" customHeight="1" s="6"/>
+    <row r="159" ht="15" customHeight="1" s="6"/>
+    <row r="160" ht="15" customHeight="1" s="6"/>
+    <row r="161" ht="15" customHeight="1" s="6"/>
+    <row r="162" ht="15" customHeight="1" s="6"/>
+    <row r="163" ht="15" customHeight="1" s="6"/>
+    <row r="164" ht="15" customHeight="1" s="6"/>
+    <row r="165" ht="15" customHeight="1" s="6"/>
+    <row r="166" ht="15" customHeight="1" s="6"/>
+    <row r="167" ht="15" customHeight="1" s="6"/>
+    <row r="168" ht="15" customHeight="1" s="6"/>
+    <row r="169" ht="15" customHeight="1" s="6"/>
+    <row r="170" ht="15" customHeight="1" s="6"/>
+    <row r="171" ht="15" customHeight="1" s="6"/>
+    <row r="172" ht="15" customHeight="1" s="6"/>
+    <row r="173" ht="15" customHeight="1" s="6"/>
+    <row r="174" ht="15" customHeight="1" s="6"/>
+    <row r="175" ht="15" customHeight="1" s="6"/>
+    <row r="176" ht="15" customHeight="1" s="6"/>
+    <row r="177" ht="15" customHeight="1" s="6"/>
+    <row r="178" ht="15" customHeight="1" s="6"/>
+    <row r="179" ht="15" customHeight="1" s="6"/>
+    <row r="180" ht="15" customHeight="1" s="6"/>
+    <row r="181" ht="15" customHeight="1" s="6"/>
+    <row r="182" ht="15" customHeight="1" s="6"/>
+    <row r="183" ht="15" customHeight="1" s="6"/>
+    <row r="184" ht="15" customHeight="1" s="6"/>
+    <row r="185" ht="15" customHeight="1" s="6"/>
+    <row r="186" ht="15" customHeight="1" s="6"/>
+    <row r="187" ht="15" customHeight="1" s="6"/>
+    <row r="188" ht="15" customHeight="1" s="6"/>
+    <row r="189" ht="15" customHeight="1" s="6"/>
+    <row r="190" ht="15" customHeight="1" s="6"/>
+    <row r="191" ht="15" customHeight="1" s="6"/>
+    <row r="192" ht="15" customHeight="1" s="6"/>
+    <row r="193" ht="15" customHeight="1" s="6"/>
+    <row r="194" ht="15" customHeight="1" s="6"/>
+    <row r="195" ht="15" customHeight="1" s="6"/>
+    <row r="196" ht="15" customHeight="1" s="6"/>
+    <row r="197" ht="15" customHeight="1" s="6"/>
+    <row r="198" ht="15" customHeight="1" s="6"/>
+    <row r="199" ht="15" customHeight="1" s="6"/>
+    <row r="200" ht="15" customHeight="1" s="6"/>
+    <row r="201" ht="15" customHeight="1" s="6"/>
+    <row r="202" ht="15" customHeight="1" s="6"/>
+    <row r="203" ht="15" customHeight="1" s="6"/>
+    <row r="204" ht="15" customHeight="1" s="6"/>
+    <row r="205" ht="15" customHeight="1" s="6"/>
+    <row r="206" ht="15" customHeight="1" s="6"/>
+    <row r="207" ht="15" customHeight="1" s="6"/>
+    <row r="208" ht="15" customHeight="1" s="6"/>
+    <row r="209" ht="15" customHeight="1" s="6"/>
+    <row r="210" ht="15" customHeight="1" s="6"/>
+    <row r="211" ht="15" customHeight="1" s="6"/>
+    <row r="212" ht="15" customHeight="1" s="6"/>
+    <row r="213" ht="15" customHeight="1" s="6"/>
+    <row r="214" ht="15" customHeight="1" s="6"/>
+    <row r="215" ht="15" customHeight="1" s="6"/>
+    <row r="216" ht="15" customHeight="1" s="6"/>
+    <row r="217" ht="15" customHeight="1" s="6"/>
+    <row r="218" ht="15" customHeight="1" s="6"/>
+    <row r="219" ht="15" customHeight="1" s="6"/>
+    <row r="220" ht="15" customHeight="1" s="6"/>
+    <row r="221" ht="15" customHeight="1" s="6"/>
+    <row r="222" ht="15" customHeight="1" s="6"/>
+    <row r="223" ht="15" customHeight="1" s="6"/>
+    <row r="224" ht="15" customHeight="1" s="6"/>
+    <row r="225" ht="15" customHeight="1" s="6"/>
+    <row r="226" ht="15" customHeight="1" s="6"/>
+    <row r="227" ht="15" customHeight="1" s="6"/>
+    <row r="228" ht="15" customHeight="1" s="6"/>
+    <row r="229" ht="15" customHeight="1" s="6"/>
+    <row r="230" ht="15" customHeight="1" s="6"/>
+    <row r="231" ht="15" customHeight="1" s="6"/>
+    <row r="232" ht="15" customHeight="1" s="6"/>
+    <row r="233" ht="15" customHeight="1" s="6"/>
+    <row r="234" ht="15" customHeight="1" s="6"/>
+    <row r="235" ht="15" customHeight="1" s="6"/>
+    <row r="236" ht="15" customHeight="1" s="6"/>
+    <row r="237" ht="15" customHeight="1" s="6"/>
+    <row r="238" ht="15" customHeight="1" s="6"/>
+    <row r="239" ht="15" customHeight="1" s="6"/>
+    <row r="240" ht="15" customHeight="1" s="6"/>
+    <row r="241" ht="15" customHeight="1" s="6"/>
+    <row r="242" ht="15" customHeight="1" s="6"/>
+    <row r="243" ht="15" customHeight="1" s="6"/>
+    <row r="244" ht="15" customHeight="1" s="6"/>
+    <row r="245" ht="15" customHeight="1" s="6"/>
+    <row r="246" ht="15" customHeight="1" s="6"/>
+    <row r="247" ht="15" customHeight="1" s="6"/>
+    <row r="248" ht="15" customHeight="1" s="6"/>
+    <row r="249" ht="15" customHeight="1" s="6"/>
+    <row r="250" ht="15" customHeight="1" s="6"/>
+    <row r="251" ht="15" customHeight="1" s="6"/>
+    <row r="252" ht="15" customHeight="1" s="6"/>
+    <row r="253" ht="15" customHeight="1" s="6"/>
+    <row r="254" ht="15" customHeight="1" s="6"/>
+    <row r="255" ht="15" customHeight="1" s="6"/>
+    <row r="256" ht="15" customHeight="1" s="6"/>
+    <row r="257" ht="15" customHeight="1" s="6"/>
+    <row r="258" ht="15" customHeight="1" s="6"/>
+    <row r="259" ht="15" customHeight="1" s="6"/>
+    <row r="260" ht="15" customHeight="1" s="6"/>
+    <row r="261" ht="15" customHeight="1" s="6"/>
+    <row r="262" ht="15" customHeight="1" s="6"/>
+    <row r="263" ht="15" customHeight="1" s="6"/>
+    <row r="264" ht="15" customHeight="1" s="6"/>
+    <row r="265" ht="15" customHeight="1" s="6"/>
+    <row r="266" ht="15" customHeight="1" s="6"/>
+    <row r="267" ht="15" customHeight="1" s="6"/>
+    <row r="268" ht="15" customHeight="1" s="6"/>
+    <row r="269" ht="15" customHeight="1" s="6"/>
+    <row r="270" ht="15" customHeight="1" s="6"/>
+    <row r="271" ht="15" customHeight="1" s="6"/>
+    <row r="272" ht="15" customHeight="1" s="6"/>
+    <row r="273" ht="15" customHeight="1" s="6"/>
+    <row r="274" ht="15" customHeight="1" s="6"/>
+    <row r="275" ht="15" customHeight="1" s="6"/>
+    <row r="276" ht="15" customHeight="1" s="6"/>
+    <row r="277" ht="15" customHeight="1" s="6"/>
+    <row r="278" ht="15" customHeight="1" s="6"/>
+    <row r="279" ht="15" customHeight="1" s="6"/>
+    <row r="280" ht="15" customHeight="1" s="6"/>
+    <row r="281" ht="15" customHeight="1" s="6"/>
+    <row r="282" ht="15" customHeight="1" s="6"/>
+    <row r="283" ht="15" customHeight="1" s="6"/>
+    <row r="284" ht="15" customHeight="1" s="6"/>
+    <row r="285" ht="15" customHeight="1" s="6"/>
+    <row r="286" ht="15" customHeight="1" s="6"/>
+    <row r="287" ht="15" customHeight="1" s="6"/>
+    <row r="288" ht="15" customHeight="1" s="6"/>
+    <row r="289" ht="15" customHeight="1" s="6"/>
+    <row r="290" ht="15" customHeight="1" s="6"/>
+    <row r="291" ht="15" customHeight="1" s="6"/>
+    <row r="292" ht="15" customHeight="1" s="6"/>
+    <row r="293" ht="15" customHeight="1" s="6"/>
+    <row r="294" ht="15" customHeight="1" s="6"/>
+    <row r="295" ht="15" customHeight="1" s="6"/>
+    <row r="296" ht="15" customHeight="1" s="6"/>
+    <row r="297" ht="15" customHeight="1" s="6"/>
+    <row r="298" ht="15" customHeight="1" s="6"/>
+    <row r="299" ht="15" customHeight="1" s="6"/>
+    <row r="300" ht="15" customHeight="1" s="6"/>
+    <row r="301" ht="15" customHeight="1" s="6"/>
+    <row r="302" ht="15" customHeight="1" s="6"/>
+    <row r="303" ht="15" customHeight="1" s="6"/>
+    <row r="304" ht="15" customHeight="1" s="6"/>
+    <row r="305" ht="15" customHeight="1" s="6"/>
+    <row r="306" ht="15" customHeight="1" s="6"/>
+    <row r="307" ht="15" customHeight="1" s="6"/>
+    <row r="308" ht="15" customHeight="1" s="6"/>
+    <row r="309" ht="15" customHeight="1" s="6"/>
+    <row r="310" ht="15" customHeight="1" s="6"/>
+    <row r="311" ht="15" customHeight="1" s="6"/>
+    <row r="312" ht="15" customHeight="1" s="6"/>
+    <row r="313" ht="15" customHeight="1" s="6"/>
+    <row r="314" ht="15" customHeight="1" s="6"/>
+    <row r="315" ht="15" customHeight="1" s="6"/>
+    <row r="316" ht="15" customHeight="1" s="6"/>
+    <row r="317" ht="15" customHeight="1" s="6"/>
+    <row r="318" ht="15" customHeight="1" s="6"/>
+    <row r="319" ht="15" customHeight="1" s="6"/>
+    <row r="320" ht="15" customHeight="1" s="6"/>
+    <row r="321" ht="15" customHeight="1" s="6"/>
+    <row r="322" ht="15" customHeight="1" s="6"/>
+    <row r="323" ht="15" customHeight="1" s="6"/>
+    <row r="324" ht="15" customHeight="1" s="6"/>
+    <row r="325" ht="15" customHeight="1" s="6"/>
+    <row r="326" ht="15" customHeight="1" s="6"/>
+    <row r="327" ht="15" customHeight="1" s="6"/>
+    <row r="328" ht="15" customHeight="1" s="6"/>
+    <row r="329" ht="15" customHeight="1" s="6"/>
+    <row r="330" ht="15" customHeight="1" s="6"/>
+    <row r="331" ht="15" customHeight="1" s="6"/>
+    <row r="332" ht="15" customHeight="1" s="6"/>
+    <row r="333" ht="15" customHeight="1" s="6"/>
+    <row r="334" ht="15" customHeight="1" s="6"/>
+    <row r="335" ht="15" customHeight="1" s="6"/>
+    <row r="336" ht="15" customHeight="1" s="6"/>
+    <row r="337" ht="15" customHeight="1" s="6"/>
+    <row r="338" ht="15" customHeight="1" s="6"/>
+    <row r="339" ht="15" customHeight="1" s="6"/>
+    <row r="340" ht="15" customHeight="1" s="6"/>
+    <row r="341" ht="15" customHeight="1" s="6"/>
+    <row r="342" ht="15" customHeight="1" s="6"/>
+    <row r="343" ht="15" customHeight="1" s="6"/>
+    <row r="344" ht="15" customHeight="1" s="6"/>
+    <row r="345" ht="15" customHeight="1" s="6"/>
+    <row r="346" ht="15" customHeight="1" s="6"/>
+    <row r="347" ht="15" customHeight="1" s="6"/>
+    <row r="348" ht="15" customHeight="1" s="6"/>
+    <row r="349" ht="15" customHeight="1" s="6"/>
+    <row r="350" ht="15" customHeight="1" s="6"/>
+    <row r="351" ht="15" customHeight="1" s="6"/>
+    <row r="352" ht="15" customHeight="1" s="6"/>
+    <row r="353" ht="15" customHeight="1" s="6"/>
+    <row r="354" ht="15" customHeight="1" s="6"/>
+    <row r="355" ht="15" customHeight="1" s="6"/>
+    <row r="356" ht="15" customHeight="1" s="6"/>
+    <row r="357" ht="15" customHeight="1" s="6"/>
+    <row r="358" ht="15" customHeight="1" s="6"/>
+    <row r="359" ht="15" customHeight="1" s="6"/>
+    <row r="360" ht="15" customHeight="1" s="6"/>
+    <row r="361" ht="15" customHeight="1" s="6"/>
+    <row r="362" ht="15" customHeight="1" s="6"/>
+    <row r="363" ht="15" customHeight="1" s="6"/>
+    <row r="364" ht="15" customHeight="1" s="6"/>
+    <row r="365" ht="15" customHeight="1" s="6"/>
+    <row r="366" ht="15" customHeight="1" s="6"/>
+    <row r="367" ht="15" customHeight="1" s="6"/>
+    <row r="368" ht="15" customHeight="1" s="6"/>
+    <row r="369" ht="15" customHeight="1" s="6"/>
+    <row r="370" ht="15" customHeight="1" s="6"/>
+    <row r="371" ht="15" customHeight="1" s="6"/>
+    <row r="372" ht="15" customHeight="1" s="6"/>
+    <row r="373" ht="15" customHeight="1" s="6"/>
+    <row r="374" ht="15" customHeight="1" s="6"/>
+    <row r="375" ht="15" customHeight="1" s="6"/>
+    <row r="376" ht="15" customHeight="1" s="6"/>
+    <row r="377" ht="15" customHeight="1" s="6"/>
+    <row r="378" ht="15" customHeight="1" s="6"/>
+    <row r="379" ht="15" customHeight="1" s="6"/>
+    <row r="380" ht="15" customHeight="1" s="6"/>
+    <row r="381" ht="15" customHeight="1" s="6"/>
+    <row r="382" ht="15" customHeight="1" s="6"/>
+    <row r="383" ht="15" customHeight="1" s="6"/>
+    <row r="384" ht="15" customHeight="1" s="6"/>
+    <row r="385" ht="15" customHeight="1" s="6"/>
+    <row r="386" ht="15" customHeight="1" s="6"/>
+    <row r="387" ht="15" customHeight="1" s="6"/>
+    <row r="388" ht="15" customHeight="1" s="6"/>
+    <row r="389" ht="15" customHeight="1" s="6"/>
+    <row r="390" ht="15" customHeight="1" s="6"/>
+    <row r="391" ht="15" customHeight="1" s="6"/>
+    <row r="392" ht="15" customHeight="1" s="6"/>
+    <row r="393" ht="15" customHeight="1" s="6"/>
+    <row r="394" ht="15" customHeight="1" s="6"/>
+    <row r="395" ht="15" customHeight="1" s="6"/>
+    <row r="396" ht="15" customHeight="1" s="6"/>
+    <row r="397" ht="15" customHeight="1" s="6"/>
+    <row r="398" ht="15" customHeight="1" s="6"/>
+    <row r="399" ht="15" customHeight="1" s="6"/>
+    <row r="400" ht="15" customHeight="1" s="6"/>
+    <row r="401" ht="15" customHeight="1" s="6"/>
+    <row r="402" ht="15" customHeight="1" s="6"/>
+    <row r="403" ht="15" customHeight="1" s="6"/>
+    <row r="404" ht="15" customHeight="1" s="6"/>
+    <row r="405" ht="15" customHeight="1" s="6"/>
+    <row r="406" ht="15" customHeight="1" s="6"/>
+    <row r="407" ht="15" customHeight="1" s="6"/>
+    <row r="408" ht="15" customHeight="1" s="6"/>
+    <row r="409" ht="15" customHeight="1" s="6"/>
+    <row r="410" ht="15" customHeight="1" s="6"/>
+    <row r="411" ht="15" customHeight="1" s="6"/>
+    <row r="412" ht="15" customHeight="1" s="6"/>
+    <row r="413" ht="15" customHeight="1" s="6"/>
+    <row r="414" ht="15" customHeight="1" s="6"/>
+    <row r="415" ht="15" customHeight="1" s="6"/>
+    <row r="416" ht="15" customHeight="1" s="6"/>
+    <row r="417" ht="15" customHeight="1" s="6"/>
+    <row r="418" ht="15" customHeight="1" s="6"/>
+    <row r="419" ht="15" customHeight="1" s="6"/>
+    <row r="420" ht="15" customHeight="1" s="6"/>
+    <row r="421" ht="15" customHeight="1" s="6"/>
+    <row r="422" ht="15" customHeight="1" s="6"/>
+    <row r="423" ht="15" customHeight="1" s="6"/>
+    <row r="424" ht="15" customHeight="1" s="6"/>
+    <row r="425" ht="15" customHeight="1" s="6"/>
+    <row r="426" ht="15" customHeight="1" s="6"/>
+    <row r="427" ht="15" customHeight="1" s="6"/>
+    <row r="428" ht="15" customHeight="1" s="6"/>
+    <row r="429" ht="15" customHeight="1" s="6"/>
+    <row r="430" ht="15" customHeight="1" s="6"/>
+    <row r="431" ht="15" customHeight="1" s="6"/>
+    <row r="432" ht="15" customHeight="1" s="6"/>
+    <row r="433" ht="15" customHeight="1" s="6"/>
+    <row r="434" ht="15" customHeight="1" s="6"/>
+    <row r="435" ht="15" customHeight="1" s="6"/>
+    <row r="436" ht="15" customHeight="1" s="6"/>
+    <row r="437" ht="15" customHeight="1" s="6"/>
+    <row r="438" ht="15" customHeight="1" s="6"/>
+    <row r="439" ht="15" customHeight="1" s="6"/>
+    <row r="440" ht="15" customHeight="1" s="6"/>
+    <row r="441" ht="15" customHeight="1" s="6"/>
+    <row r="442" ht="15" customHeight="1" s="6"/>
+    <row r="443" ht="15" customHeight="1" s="6"/>
+    <row r="444" ht="15" customHeight="1" s="6"/>
+    <row r="445" ht="15" customHeight="1" s="6"/>
+    <row r="446" ht="15" customHeight="1" s="6"/>
+    <row r="447" ht="15" customHeight="1" s="6"/>
+    <row r="448" ht="15" customHeight="1" s="6"/>
+    <row r="449" ht="15" customHeight="1" s="6"/>
+    <row r="450" ht="15" customHeight="1" s="6"/>
+    <row r="451" ht="15" customHeight="1" s="6"/>
+    <row r="452" ht="15" customHeight="1" s="6"/>
+    <row r="453" ht="15" customHeight="1" s="6"/>
+    <row r="454" ht="15" customHeight="1" s="6"/>
+    <row r="455" ht="15" customHeight="1" s="6"/>
+    <row r="456" ht="15" customHeight="1" s="6"/>
+    <row r="457" ht="15" customHeight="1" s="6"/>
+    <row r="458" ht="15" customHeight="1" s="6"/>
+    <row r="459" ht="15" customHeight="1" s="6"/>
+    <row r="460" ht="15" customHeight="1" s="6"/>
+    <row r="461" ht="15" customHeight="1" s="6"/>
+    <row r="462" ht="15" customHeight="1" s="6"/>
+    <row r="463" ht="15" customHeight="1" s="6"/>
+    <row r="464" ht="15" customHeight="1" s="6"/>
+    <row r="465" ht="15" customHeight="1" s="6"/>
+    <row r="466" ht="15" customHeight="1" s="6"/>
+    <row r="467" ht="15" customHeight="1" s="6"/>
+    <row r="468" ht="15" customHeight="1" s="6"/>
+    <row r="469" ht="15" customHeight="1" s="6"/>
+    <row r="470" ht="15" customHeight="1" s="6"/>
+    <row r="471" ht="15" customHeight="1" s="6"/>
+    <row r="472" ht="15" customHeight="1" s="6"/>
+    <row r="473" ht="15" customHeight="1" s="6"/>
+    <row r="474" ht="15" customHeight="1" s="6"/>
+    <row r="475" ht="15" customHeight="1" s="6"/>
+    <row r="476" ht="15" customHeight="1" s="6"/>
+    <row r="477" ht="15" customHeight="1" s="6"/>
+    <row r="478" ht="15" customHeight="1" s="6"/>
+    <row r="479" ht="15" customHeight="1" s="6"/>
+    <row r="480" ht="15" customHeight="1" s="6"/>
+    <row r="481" ht="15" customHeight="1" s="6"/>
+    <row r="482" ht="15" customHeight="1" s="6"/>
+    <row r="483" ht="15" customHeight="1" s="6"/>
+    <row r="484" ht="15" customHeight="1" s="6"/>
+    <row r="485" ht="15" customHeight="1" s="6"/>
+    <row r="486" ht="15" customHeight="1" s="6"/>
+    <row r="487" ht="15" customHeight="1" s="6"/>
+    <row r="488" ht="15" customHeight="1" s="6"/>
+    <row r="489" ht="15" customHeight="1" s="6"/>
+    <row r="490" ht="15" customHeight="1" s="6"/>
+    <row r="491" ht="15" customHeight="1" s="6"/>
+    <row r="492" ht="15" customHeight="1" s="6"/>
+    <row r="493" ht="15" customHeight="1" s="6"/>
+    <row r="494" ht="15" customHeight="1" s="6"/>
+    <row r="495" ht="15" customHeight="1" s="6"/>
+    <row r="496" ht="15" customHeight="1" s="6"/>
+    <row r="497" ht="15" customHeight="1" s="6"/>
+    <row r="498" ht="15" customHeight="1" s="6"/>
+    <row r="499" ht="15" customHeight="1" s="6"/>
+    <row r="500" ht="15" customHeight="1" s="6"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>